<commit_message>
set all dry rates to 0
</commit_message>
<xml_diff>
--- a/db/passport.xlsx
+++ b/db/passport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daigo\Documents\WPy64-3741\notebooks\docs\boatms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daigo\Documents\WPy64-3741\notebooks\spyder\tms-load-robot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -705,7 +705,7 @@
   <dimension ref="A1:W106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5981,64 +5981,64 @@
         <v>69</v>
       </c>
       <c r="D75" s="10">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="E75" s="10">
-        <v>430</v>
-      </c>
-      <c r="F75" s="5">
-        <v>550</v>
+        <v>0</v>
+      </c>
+      <c r="F75" s="10">
+        <v>0</v>
       </c>
       <c r="G75" s="10">
-        <v>570</v>
+        <v>0</v>
       </c>
       <c r="H75" s="10">
-        <v>590</v>
+        <v>0</v>
       </c>
       <c r="I75" s="10">
-        <v>590</v>
+        <v>0</v>
       </c>
       <c r="J75" s="10">
-        <v>590</v>
+        <v>0</v>
       </c>
       <c r="K75" s="10">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="L75" s="10">
-        <v>705</v>
+        <v>0</v>
       </c>
       <c r="M75" s="10">
-        <v>765</v>
+        <v>0</v>
       </c>
       <c r="N75" s="10">
-        <v>820</v>
+        <v>0</v>
       </c>
       <c r="O75" s="10">
-        <v>875</v>
+        <v>0</v>
       </c>
       <c r="P75" s="10">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="Q75" s="10">
-        <v>930</v>
+        <v>0</v>
       </c>
       <c r="R75" s="10">
-        <v>955</v>
+        <v>0</v>
       </c>
       <c r="S75" s="10">
-        <v>985</v>
+        <v>0</v>
       </c>
       <c r="T75" s="10">
-        <v>1010</v>
+        <v>0</v>
       </c>
       <c r="U75" s="10">
-        <v>1035</v>
+        <v>0</v>
       </c>
       <c r="V75" s="10">
-        <v>1095</v>
+        <v>0</v>
       </c>
       <c r="W75" s="10">
-        <v>1150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.25">
@@ -6052,64 +6052,64 @@
         <v>69</v>
       </c>
       <c r="D76" s="10">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="E76" s="10">
-        <v>445</v>
-      </c>
-      <c r="F76" s="5">
-        <v>525</v>
+        <v>0</v>
+      </c>
+      <c r="F76" s="10">
+        <v>0</v>
       </c>
       <c r="G76" s="10">
-        <v>570</v>
+        <v>0</v>
       </c>
       <c r="H76" s="10">
-        <v>590</v>
+        <v>0</v>
       </c>
       <c r="I76" s="10">
-        <v>590</v>
+        <v>0</v>
       </c>
       <c r="J76" s="10">
-        <v>590</v>
+        <v>0</v>
       </c>
       <c r="K76" s="10">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="L76" s="10">
-        <v>705</v>
+        <v>0</v>
       </c>
       <c r="M76" s="10">
-        <v>765</v>
+        <v>0</v>
       </c>
       <c r="N76" s="10">
-        <v>820</v>
+        <v>0</v>
       </c>
       <c r="O76" s="10">
-        <v>875</v>
+        <v>0</v>
       </c>
       <c r="P76" s="10">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="Q76" s="10">
-        <v>930</v>
+        <v>0</v>
       </c>
       <c r="R76" s="10">
-        <v>955</v>
+        <v>0</v>
       </c>
       <c r="S76" s="10">
-        <v>985</v>
+        <v>0</v>
       </c>
       <c r="T76" s="10">
-        <v>1010</v>
+        <v>0</v>
       </c>
       <c r="U76" s="10">
-        <v>1035</v>
+        <v>0</v>
       </c>
       <c r="V76" s="10">
-        <v>1095</v>
+        <v>0</v>
       </c>
       <c r="W76" s="10">
-        <v>1150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.25">
@@ -6123,64 +6123,64 @@
         <v>69</v>
       </c>
       <c r="D77" s="10">
-        <v>235</v>
+        <v>0</v>
       </c>
       <c r="E77" s="10">
-        <v>370</v>
-      </c>
-      <c r="F77" s="5">
-        <v>385</v>
+        <v>0</v>
+      </c>
+      <c r="F77" s="10">
+        <v>0</v>
       </c>
       <c r="G77" s="10">
-        <v>540</v>
+        <v>0</v>
       </c>
       <c r="H77" s="10">
-        <v>535</v>
+        <v>0</v>
       </c>
       <c r="I77" s="10">
-        <v>535</v>
+        <v>0</v>
       </c>
       <c r="J77" s="10">
-        <v>550</v>
+        <v>0</v>
       </c>
       <c r="K77" s="10">
-        <v>555</v>
+        <v>0</v>
       </c>
       <c r="L77" s="10">
-        <v>565</v>
+        <v>0</v>
       </c>
       <c r="M77" s="10">
-        <v>575</v>
+        <v>0</v>
       </c>
       <c r="N77" s="10">
-        <v>585</v>
+        <v>0</v>
       </c>
       <c r="O77" s="10">
-        <v>585</v>
+        <v>0</v>
       </c>
       <c r="P77" s="10">
-        <v>580</v>
+        <v>0</v>
       </c>
       <c r="Q77" s="10">
-        <v>580</v>
+        <v>0</v>
       </c>
       <c r="R77" s="10">
-        <v>580</v>
+        <v>0</v>
       </c>
       <c r="S77" s="10">
-        <v>580</v>
+        <v>0</v>
       </c>
       <c r="T77" s="10">
-        <v>580</v>
+        <v>0</v>
       </c>
       <c r="U77" s="10">
-        <v>580</v>
+        <v>0</v>
       </c>
       <c r="V77" s="10">
-        <v>580</v>
+        <v>0</v>
       </c>
       <c r="W77" s="10">
-        <v>580</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.25">
@@ -6194,64 +6194,64 @@
         <v>69</v>
       </c>
       <c r="D78" s="10">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="E78" s="10">
-        <v>450</v>
-      </c>
-      <c r="F78" s="5">
-        <v>540</v>
+        <v>0</v>
+      </c>
+      <c r="F78" s="10">
+        <v>0</v>
       </c>
       <c r="G78" s="10">
-        <v>570</v>
+        <v>0</v>
       </c>
       <c r="H78" s="10">
-        <v>590</v>
+        <v>0</v>
       </c>
       <c r="I78" s="10">
-        <v>590</v>
+        <v>0</v>
       </c>
       <c r="J78" s="10">
-        <v>590</v>
+        <v>0</v>
       </c>
       <c r="K78" s="10">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="L78" s="10">
-        <v>705</v>
+        <v>0</v>
       </c>
       <c r="M78" s="10">
-        <v>765</v>
+        <v>0</v>
       </c>
       <c r="N78" s="10">
-        <v>820</v>
+        <v>0</v>
       </c>
       <c r="O78" s="10">
-        <v>875</v>
+        <v>0</v>
       </c>
       <c r="P78" s="10">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="Q78" s="10">
-        <v>930</v>
+        <v>0</v>
       </c>
       <c r="R78" s="10">
-        <v>955</v>
+        <v>0</v>
       </c>
       <c r="S78" s="10">
-        <v>985</v>
+        <v>0</v>
       </c>
       <c r="T78" s="10">
-        <v>1010</v>
+        <v>0</v>
       </c>
       <c r="U78" s="10">
-        <v>1035</v>
+        <v>0</v>
       </c>
       <c r="V78" s="10">
-        <v>1095</v>
+        <v>0</v>
       </c>
       <c r="W78" s="10">
-        <v>1150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
@@ -6265,64 +6265,64 @@
         <v>69</v>
       </c>
       <c r="D79" s="10">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E79" s="10">
-        <v>105</v>
-      </c>
-      <c r="F79" s="5">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="F79" s="10">
+        <v>0</v>
       </c>
       <c r="G79" s="10">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="H79" s="10">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="I79" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="J79" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="K79" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="L79" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="M79" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="N79" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="O79" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="P79" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="Q79" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="R79" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="S79" s="10">
-        <v>325</v>
+        <v>0</v>
       </c>
       <c r="T79" s="10">
-        <v>325</v>
+        <v>0</v>
       </c>
       <c r="U79" s="10">
-        <v>325</v>
+        <v>0</v>
       </c>
       <c r="V79" s="10">
-        <v>325</v>
+        <v>0</v>
       </c>
       <c r="W79" s="10">
-        <v>325</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.25">
@@ -6336,64 +6336,64 @@
         <v>69</v>
       </c>
       <c r="D80" s="10">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E80" s="10">
-        <v>105</v>
-      </c>
-      <c r="F80" s="5">
-        <v>145</v>
+        <v>0</v>
+      </c>
+      <c r="F80" s="10">
+        <v>0</v>
       </c>
       <c r="G80" s="10">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="H80" s="10">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="I80" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="J80" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="K80" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="L80" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="M80" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="N80" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="O80" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="P80" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="Q80" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="R80" s="10">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="S80" s="10">
-        <v>325</v>
+        <v>0</v>
       </c>
       <c r="T80" s="10">
-        <v>325</v>
+        <v>0</v>
       </c>
       <c r="U80" s="10">
-        <v>325</v>
+        <v>0</v>
       </c>
       <c r="V80" s="10">
-        <v>325</v>
+        <v>0</v>
       </c>
       <c r="W80" s="10">
-        <v>325</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.25">
@@ -6407,57 +6407,65 @@
         <v>69</v>
       </c>
       <c r="D81" s="10">
-        <v>355</v>
+        <v>0</v>
       </c>
       <c r="E81" s="10">
-        <v>635</v>
-      </c>
-      <c r="F81" s="5">
-        <v>835</v>
+        <v>0</v>
+      </c>
+      <c r="F81" s="10">
+        <v>0</v>
       </c>
       <c r="G81" s="10">
-        <v>925</v>
+        <v>0</v>
       </c>
       <c r="H81" s="10">
-        <v>1035</v>
+        <v>0</v>
       </c>
       <c r="I81" s="10">
-        <v>1240</v>
+        <v>0</v>
       </c>
       <c r="J81" s="10">
-        <v>1400</v>
+        <v>0</v>
       </c>
       <c r="K81" s="10">
-        <v>1600</v>
+        <v>0</v>
       </c>
       <c r="L81" s="10">
-        <v>1740</v>
+        <v>0</v>
       </c>
       <c r="M81" s="10">
-        <v>1935</v>
+        <v>0</v>
       </c>
       <c r="N81" s="10">
-        <v>2040</v>
+        <v>0</v>
       </c>
       <c r="O81" s="10">
-        <v>2160</v>
+        <v>0</v>
       </c>
       <c r="P81" s="10">
-        <v>2265</v>
+        <v>0</v>
       </c>
       <c r="Q81" s="10">
-        <v>2380</v>
+        <v>0</v>
       </c>
       <c r="R81" s="10">
-        <v>2485</v>
+        <v>0</v>
       </c>
       <c r="S81" s="10">
-        <v>2600</v>
-      </c>
-      <c r="T81" s="5"/>
-      <c r="U81" s="5"/>
-      <c r="V81" s="5"/>
-      <c r="W81" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="T81" s="10">
+        <v>0</v>
+      </c>
+      <c r="U81" s="10">
+        <v>0</v>
+      </c>
+      <c r="V81" s="10">
+        <v>0</v>
+      </c>
+      <c r="W81" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
@@ -6470,64 +6478,64 @@
         <v>69</v>
       </c>
       <c r="D82" s="10">
-        <v>420</v>
+        <v>0</v>
       </c>
       <c r="E82" s="10">
-        <v>660</v>
-      </c>
-      <c r="F82" s="5">
-        <v>985</v>
+        <v>0</v>
+      </c>
+      <c r="F82" s="10">
+        <v>0</v>
       </c>
       <c r="G82" s="10">
-        <v>1190</v>
+        <v>0</v>
       </c>
       <c r="H82" s="10">
-        <v>1475</v>
+        <v>0</v>
       </c>
       <c r="I82" s="10">
-        <v>1770</v>
+        <v>0</v>
       </c>
       <c r="J82" s="10">
-        <v>2060</v>
+        <v>0</v>
       </c>
       <c r="K82" s="10">
-        <v>2350</v>
+        <v>0</v>
       </c>
       <c r="L82" s="10">
-        <v>2635</v>
+        <v>0</v>
       </c>
       <c r="M82" s="10">
-        <v>2925</v>
+        <v>0</v>
       </c>
       <c r="N82" s="10">
-        <v>3205</v>
+        <v>0</v>
       </c>
       <c r="O82" s="10">
-        <v>3495</v>
+        <v>0</v>
       </c>
       <c r="P82" s="10">
-        <v>3770</v>
+        <v>0</v>
       </c>
       <c r="Q82" s="10">
-        <v>4060</v>
+        <v>0</v>
       </c>
       <c r="R82" s="10">
-        <v>4335</v>
+        <v>0</v>
       </c>
       <c r="S82" s="10">
-        <v>4620</v>
+        <v>0</v>
       </c>
       <c r="T82" s="10">
-        <v>4890</v>
+        <v>0</v>
       </c>
       <c r="U82" s="10">
-        <v>5175</v>
+        <v>0</v>
       </c>
       <c r="V82" s="10">
-        <v>5465</v>
+        <v>0</v>
       </c>
       <c r="W82" s="10">
-        <v>5750</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.25">
@@ -6541,64 +6549,64 @@
         <v>69</v>
       </c>
       <c r="D83" s="10">
-        <v>420</v>
+        <v>0</v>
       </c>
       <c r="E83" s="10">
-        <v>660</v>
-      </c>
-      <c r="F83" s="5">
-        <v>985</v>
+        <v>0</v>
+      </c>
+      <c r="F83" s="10">
+        <v>0</v>
       </c>
       <c r="G83" s="10">
-        <v>1190</v>
+        <v>0</v>
       </c>
       <c r="H83" s="10">
-        <v>1475</v>
+        <v>0</v>
       </c>
       <c r="I83" s="10">
-        <v>1770</v>
+        <v>0</v>
       </c>
       <c r="J83" s="10">
-        <v>2060</v>
+        <v>0</v>
       </c>
       <c r="K83" s="10">
-        <v>2350</v>
+        <v>0</v>
       </c>
       <c r="L83" s="10">
-        <v>2635</v>
+        <v>0</v>
       </c>
       <c r="M83" s="10">
-        <v>2925</v>
+        <v>0</v>
       </c>
       <c r="N83" s="10">
-        <v>3205</v>
+        <v>0</v>
       </c>
       <c r="O83" s="10">
-        <v>3495</v>
+        <v>0</v>
       </c>
       <c r="P83" s="10">
-        <v>3770</v>
+        <v>0</v>
       </c>
       <c r="Q83" s="10">
-        <v>4060</v>
+        <v>0</v>
       </c>
       <c r="R83" s="10">
-        <v>4335</v>
+        <v>0</v>
       </c>
       <c r="S83" s="10">
-        <v>4620</v>
+        <v>0</v>
       </c>
       <c r="T83" s="10">
-        <v>4890</v>
+        <v>0</v>
       </c>
       <c r="U83" s="10">
-        <v>5175</v>
+        <v>0</v>
       </c>
       <c r="V83" s="10">
-        <v>5465</v>
+        <v>0</v>
       </c>
       <c r="W83" s="10">
-        <v>5750</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.25">
@@ -6612,64 +6620,64 @@
         <v>69</v>
       </c>
       <c r="D84" s="10">
-        <v>440</v>
+        <v>0</v>
       </c>
       <c r="E84" s="10">
-        <v>725</v>
-      </c>
-      <c r="F84" s="5">
-        <v>800</v>
+        <v>0</v>
+      </c>
+      <c r="F84" s="10">
+        <v>0</v>
       </c>
       <c r="G84" s="10">
-        <v>840</v>
+        <v>0</v>
       </c>
       <c r="H84" s="10">
-        <v>860</v>
+        <v>0</v>
       </c>
       <c r="I84" s="10">
-        <v>1030</v>
+        <v>0</v>
       </c>
       <c r="J84" s="10">
-        <v>1195</v>
+        <v>0</v>
       </c>
       <c r="K84" s="10">
-        <v>1365</v>
+        <v>0</v>
       </c>
       <c r="L84" s="10">
-        <v>1530</v>
+        <v>0</v>
       </c>
       <c r="M84" s="10">
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="N84" s="10">
-        <v>1860</v>
+        <v>0</v>
       </c>
       <c r="O84" s="10">
-        <v>2030</v>
+        <v>0</v>
       </c>
       <c r="P84" s="10">
-        <v>2190</v>
+        <v>0</v>
       </c>
       <c r="Q84" s="10">
-        <v>2355</v>
+        <v>0</v>
       </c>
       <c r="R84" s="10">
-        <v>2515</v>
+        <v>0</v>
       </c>
       <c r="S84" s="10">
-        <v>2680</v>
+        <v>0</v>
       </c>
       <c r="T84" s="10">
-        <v>2835</v>
+        <v>0</v>
       </c>
       <c r="U84" s="10">
-        <v>3005</v>
+        <v>0</v>
       </c>
       <c r="V84" s="10">
-        <v>3170</v>
+        <v>0</v>
       </c>
       <c r="W84" s="10">
-        <v>3335</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.25">
@@ -6683,64 +6691,64 @@
         <v>69</v>
       </c>
       <c r="D85" s="10">
-        <v>460</v>
+        <v>0</v>
       </c>
       <c r="E85" s="10">
-        <v>750</v>
-      </c>
-      <c r="F85" s="5">
-        <v>800</v>
+        <v>0</v>
+      </c>
+      <c r="F85" s="10">
+        <v>0</v>
       </c>
       <c r="G85" s="10">
-        <v>840</v>
+        <v>0</v>
       </c>
       <c r="H85" s="10">
-        <v>860</v>
+        <v>0</v>
       </c>
       <c r="I85" s="10">
-        <v>1030</v>
+        <v>0</v>
       </c>
       <c r="J85" s="10">
-        <v>1195</v>
+        <v>0</v>
       </c>
       <c r="K85" s="10">
-        <v>1365</v>
+        <v>0</v>
       </c>
       <c r="L85" s="10">
-        <v>1530</v>
+        <v>0</v>
       </c>
       <c r="M85" s="10">
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="N85" s="10">
-        <v>1860</v>
+        <v>0</v>
       </c>
       <c r="O85" s="10">
-        <v>2030</v>
+        <v>0</v>
       </c>
       <c r="P85" s="10">
-        <v>2190</v>
+        <v>0</v>
       </c>
       <c r="Q85" s="10">
-        <v>2355</v>
+        <v>0</v>
       </c>
       <c r="R85" s="10">
-        <v>2515</v>
+        <v>0</v>
       </c>
       <c r="S85" s="10">
-        <v>2680</v>
+        <v>0</v>
       </c>
       <c r="T85" s="10">
-        <v>2835</v>
+        <v>0</v>
       </c>
       <c r="U85" s="10">
-        <v>3005</v>
+        <v>0</v>
       </c>
       <c r="V85" s="10">
-        <v>3170</v>
+        <v>0</v>
       </c>
       <c r="W85" s="10">
-        <v>3335</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.25">
@@ -6754,64 +6762,64 @@
         <v>69</v>
       </c>
       <c r="D86" s="10">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="E86" s="10">
-        <v>750</v>
-      </c>
-      <c r="F86" s="5">
-        <v>895</v>
+        <v>0</v>
+      </c>
+      <c r="F86" s="10">
+        <v>0</v>
       </c>
       <c r="G86" s="10">
-        <v>1045</v>
+        <v>0</v>
       </c>
       <c r="H86" s="10">
-        <v>1180</v>
+        <v>0</v>
       </c>
       <c r="I86" s="10">
-        <v>1300</v>
+        <v>0</v>
       </c>
       <c r="J86" s="10">
-        <v>1485</v>
+        <v>0</v>
       </c>
       <c r="K86" s="10">
-        <v>1590</v>
+        <v>0</v>
       </c>
       <c r="L86" s="10">
-        <v>1640</v>
+        <v>0</v>
       </c>
       <c r="M86" s="10">
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="N86" s="10">
-        <v>1750</v>
+        <v>0</v>
       </c>
       <c r="O86" s="10">
-        <v>1810</v>
+        <v>0</v>
       </c>
       <c r="P86" s="10">
-        <v>1860</v>
+        <v>0</v>
       </c>
       <c r="Q86" s="10">
-        <v>1915</v>
+        <v>0</v>
       </c>
       <c r="R86" s="10">
-        <v>1965</v>
+        <v>0</v>
       </c>
       <c r="S86" s="10">
-        <v>2025</v>
+        <v>0</v>
       </c>
       <c r="T86" s="10">
-        <v>2070</v>
+        <v>0</v>
       </c>
       <c r="U86" s="10">
-        <v>2130</v>
+        <v>0</v>
       </c>
       <c r="V86" s="10">
-        <v>2185</v>
+        <v>0</v>
       </c>
       <c r="W86" s="10">
-        <v>2245</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:23" x14ac:dyDescent="0.25">
@@ -6825,64 +6833,64 @@
         <v>69</v>
       </c>
       <c r="D87" s="10">
-        <v>425</v>
+        <v>0</v>
       </c>
       <c r="E87" s="10">
-        <v>695</v>
-      </c>
-      <c r="F87" s="5">
-        <v>750</v>
+        <v>0</v>
+      </c>
+      <c r="F87" s="10">
+        <v>0</v>
       </c>
       <c r="G87" s="10">
-        <v>895</v>
+        <v>0</v>
       </c>
       <c r="H87" s="10">
-        <v>1035</v>
+        <v>0</v>
       </c>
       <c r="I87" s="10">
-        <v>1180</v>
+        <v>0</v>
       </c>
       <c r="J87" s="10">
-        <v>1295</v>
+        <v>0</v>
       </c>
       <c r="K87" s="10">
-        <v>1485</v>
+        <v>0</v>
       </c>
       <c r="L87" s="10">
-        <v>1580</v>
+        <v>0</v>
       </c>
       <c r="M87" s="10">
-        <v>1640</v>
+        <v>0</v>
       </c>
       <c r="N87" s="10">
-        <v>1690</v>
+        <v>0</v>
       </c>
       <c r="O87" s="10">
-        <v>1750</v>
+        <v>0</v>
       </c>
       <c r="P87" s="10">
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="Q87" s="10">
-        <v>1860</v>
+        <v>0</v>
       </c>
       <c r="R87" s="10">
-        <v>1910</v>
+        <v>0</v>
       </c>
       <c r="S87" s="10">
-        <v>1965</v>
+        <v>0</v>
       </c>
       <c r="T87" s="10">
-        <v>2015</v>
+        <v>0</v>
       </c>
       <c r="U87" s="10">
-        <v>2070</v>
+        <v>0</v>
       </c>
       <c r="V87" s="10">
-        <v>2130</v>
+        <v>0</v>
       </c>
       <c r="W87" s="10">
-        <v>2185</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.25">
@@ -6896,64 +6904,64 @@
         <v>69</v>
       </c>
       <c r="D88" s="10">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="E88" s="10">
-        <v>725</v>
-      </c>
-      <c r="F88" s="5">
-        <v>775</v>
+        <v>0</v>
+      </c>
+      <c r="F88" s="10">
+        <v>0</v>
       </c>
       <c r="G88" s="10">
-        <v>825</v>
+        <v>0</v>
       </c>
       <c r="H88" s="10">
-        <v>860</v>
+        <v>0</v>
       </c>
       <c r="I88" s="10">
-        <v>1030</v>
+        <v>0</v>
       </c>
       <c r="J88" s="10">
-        <v>1195</v>
+        <v>0</v>
       </c>
       <c r="K88" s="10">
-        <v>1365</v>
+        <v>0</v>
       </c>
       <c r="L88" s="10">
-        <v>1530</v>
+        <v>0</v>
       </c>
       <c r="M88" s="10">
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="N88" s="10">
-        <v>1860</v>
+        <v>0</v>
       </c>
       <c r="O88" s="10">
-        <v>2030</v>
+        <v>0</v>
       </c>
       <c r="P88" s="10">
-        <v>2190</v>
+        <v>0</v>
       </c>
       <c r="Q88" s="10">
-        <v>2355</v>
+        <v>0</v>
       </c>
       <c r="R88" s="10">
-        <v>2515</v>
+        <v>0</v>
       </c>
       <c r="S88" s="10">
-        <v>2680</v>
+        <v>0</v>
       </c>
       <c r="T88" s="10">
-        <v>2835</v>
+        <v>0</v>
       </c>
       <c r="U88" s="10">
-        <v>3005</v>
+        <v>0</v>
       </c>
       <c r="V88" s="10">
-        <v>3170</v>
+        <v>0</v>
       </c>
       <c r="W88" s="10">
-        <v>3335</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:23" x14ac:dyDescent="0.25">
@@ -6967,64 +6975,64 @@
         <v>69</v>
       </c>
       <c r="D89" s="10">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="E89" s="10">
-        <v>320</v>
-      </c>
-      <c r="F89" s="5">
-        <v>480</v>
+        <v>0</v>
+      </c>
+      <c r="F89" s="10">
+        <v>0</v>
       </c>
       <c r="G89" s="10">
-        <v>595</v>
+        <v>0</v>
       </c>
       <c r="H89" s="10">
-        <v>620</v>
+        <v>0</v>
       </c>
       <c r="I89" s="10">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="J89" s="10">
-        <v>680</v>
+        <v>0</v>
       </c>
       <c r="K89" s="10">
-        <v>705</v>
+        <v>0</v>
       </c>
       <c r="L89" s="10">
-        <v>735</v>
+        <v>0</v>
       </c>
       <c r="M89" s="10">
-        <v>765</v>
+        <v>0</v>
       </c>
       <c r="N89" s="10">
-        <v>790</v>
+        <v>0</v>
       </c>
       <c r="O89" s="10">
-        <v>820</v>
+        <v>0</v>
       </c>
       <c r="P89" s="10">
-        <v>845</v>
+        <v>0</v>
       </c>
       <c r="Q89" s="10">
-        <v>870</v>
+        <v>0</v>
       </c>
       <c r="R89" s="10">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="S89" s="10">
-        <v>925</v>
+        <v>0</v>
       </c>
       <c r="T89" s="10">
-        <v>950</v>
+        <v>0</v>
       </c>
       <c r="U89" s="10">
-        <v>980</v>
+        <v>0</v>
       </c>
       <c r="V89" s="10">
-        <v>1010</v>
+        <v>0</v>
       </c>
       <c r="W89" s="10">
-        <v>1035</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:23" x14ac:dyDescent="0.25">
@@ -7038,64 +7046,64 @@
         <v>69</v>
       </c>
       <c r="D90" s="10">
-        <v>315</v>
+        <v>0</v>
       </c>
       <c r="E90" s="10">
-        <v>560</v>
-      </c>
-      <c r="F90" s="5">
-        <v>840</v>
+        <v>0</v>
+      </c>
+      <c r="F90" s="10">
+        <v>0</v>
       </c>
       <c r="G90" s="10">
-        <v>1190</v>
+        <v>0</v>
       </c>
       <c r="H90" s="10">
-        <v>1180</v>
+        <v>0</v>
       </c>
       <c r="I90" s="10">
-        <v>1225</v>
+        <v>0</v>
       </c>
       <c r="J90" s="10">
-        <v>1465</v>
+        <v>0</v>
       </c>
       <c r="K90" s="10">
-        <v>1470</v>
+        <v>0</v>
       </c>
       <c r="L90" s="10">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="M90" s="10">
-        <v>1775</v>
+        <v>0</v>
       </c>
       <c r="N90" s="10">
-        <v>1785</v>
+        <v>0</v>
       </c>
       <c r="O90" s="10">
-        <v>1865</v>
+        <v>0</v>
       </c>
       <c r="P90" s="10">
-        <v>2055</v>
+        <v>0</v>
       </c>
       <c r="Q90" s="10">
-        <v>2240</v>
+        <v>0</v>
       </c>
       <c r="R90" s="10">
-        <v>2080</v>
+        <v>0</v>
       </c>
       <c r="S90" s="10">
-        <v>2255</v>
+        <v>0</v>
       </c>
       <c r="T90" s="10">
-        <v>2410</v>
+        <v>0</v>
       </c>
       <c r="U90" s="10">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="V90" s="10">
-        <v>2590</v>
+        <v>0</v>
       </c>
       <c r="W90" s="10">
-        <v>2695</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.25">
@@ -7109,61 +7117,65 @@
         <v>69</v>
       </c>
       <c r="D91" s="10">
-        <v>355</v>
+        <v>0</v>
       </c>
       <c r="E91" s="10">
-        <v>625</v>
-      </c>
-      <c r="F91" s="5">
-        <v>940</v>
+        <v>0</v>
+      </c>
+      <c r="F91" s="10">
+        <v>0</v>
       </c>
       <c r="G91" s="10">
-        <v>1190</v>
+        <v>0</v>
       </c>
       <c r="H91" s="10">
-        <v>1180</v>
+        <v>0</v>
       </c>
       <c r="I91" s="10">
-        <v>1225</v>
+        <v>0</v>
       </c>
       <c r="J91" s="10">
-        <v>1465</v>
+        <v>0</v>
       </c>
       <c r="K91" s="10">
-        <v>1470</v>
+        <v>0</v>
       </c>
       <c r="L91" s="10">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="M91" s="10">
-        <v>1775</v>
+        <v>0</v>
       </c>
       <c r="N91" s="10">
-        <v>1785</v>
+        <v>0</v>
       </c>
       <c r="O91" s="10">
-        <v>1865</v>
+        <v>0</v>
       </c>
       <c r="P91" s="10">
-        <v>2055</v>
+        <v>0</v>
       </c>
       <c r="Q91" s="10">
-        <v>2240</v>
+        <v>0</v>
       </c>
       <c r="R91" s="10">
-        <v>2080</v>
+        <v>0</v>
       </c>
       <c r="S91" s="10">
-        <v>2255</v>
+        <v>0</v>
       </c>
       <c r="T91" s="10">
-        <v>2410</v>
+        <v>0</v>
       </c>
       <c r="U91" s="10">
-        <v>2500</v>
-      </c>
-      <c r="V91" s="5"/>
-      <c r="W91" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="V91" s="10">
+        <v>0</v>
+      </c>
+      <c r="W91" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
@@ -7176,64 +7188,64 @@
         <v>69</v>
       </c>
       <c r="D92" s="10">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="E92" s="10">
-        <v>600</v>
-      </c>
-      <c r="F92" s="5">
-        <v>650</v>
+        <v>0</v>
+      </c>
+      <c r="F92" s="10">
+        <v>0</v>
       </c>
       <c r="G92" s="10">
-        <v>715</v>
+        <v>0</v>
       </c>
       <c r="H92" s="10">
-        <v>830</v>
+        <v>0</v>
       </c>
       <c r="I92" s="10">
-        <v>945</v>
+        <v>0</v>
       </c>
       <c r="J92" s="10">
-        <v>1060</v>
+        <v>0</v>
       </c>
       <c r="K92" s="10">
-        <v>1175</v>
+        <v>0</v>
       </c>
       <c r="L92" s="10">
-        <v>1260</v>
+        <v>0</v>
       </c>
       <c r="M92" s="10">
-        <v>1350</v>
+        <v>0</v>
       </c>
       <c r="N92" s="10">
-        <v>1460</v>
+        <v>0</v>
       </c>
       <c r="O92" s="10">
-        <v>1575</v>
+        <v>0</v>
       </c>
       <c r="P92" s="10">
-        <v>1685</v>
+        <v>0</v>
       </c>
       <c r="Q92" s="10">
-        <v>1770</v>
+        <v>0</v>
       </c>
       <c r="R92" s="10">
-        <v>1850</v>
+        <v>0</v>
       </c>
       <c r="S92" s="10">
-        <v>1910</v>
+        <v>0</v>
       </c>
       <c r="T92" s="10">
-        <v>1955</v>
+        <v>0</v>
       </c>
       <c r="U92" s="10">
-        <v>2070</v>
+        <v>0</v>
       </c>
       <c r="V92" s="10">
-        <v>2185</v>
+        <v>0</v>
       </c>
       <c r="W92" s="10">
-        <v>2300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:23" x14ac:dyDescent="0.25">
@@ -7247,61 +7259,65 @@
         <v>69</v>
       </c>
       <c r="D93" s="10">
-        <v>275</v>
+        <v>0</v>
       </c>
       <c r="E93" s="10">
-        <v>485</v>
-      </c>
-      <c r="F93" s="5">
-        <v>720</v>
+        <v>0</v>
+      </c>
+      <c r="F93" s="10">
+        <v>0</v>
       </c>
       <c r="G93" s="10">
-        <v>1075</v>
+        <v>0</v>
       </c>
       <c r="H93" s="10">
-        <v>1065</v>
+        <v>0</v>
       </c>
       <c r="I93" s="10">
-        <v>1065</v>
+        <v>0</v>
       </c>
       <c r="J93" s="10">
-        <v>1090</v>
+        <v>0</v>
       </c>
       <c r="K93" s="10">
-        <v>1105</v>
+        <v>0</v>
       </c>
       <c r="L93" s="10">
-        <v>1170</v>
+        <v>0</v>
       </c>
       <c r="M93" s="10">
-        <v>1335</v>
+        <v>0</v>
       </c>
       <c r="N93" s="10">
-        <v>1340</v>
+        <v>0</v>
       </c>
       <c r="O93" s="10">
-        <v>1400</v>
+        <v>0</v>
       </c>
       <c r="P93" s="10">
-        <v>1545</v>
+        <v>0</v>
       </c>
       <c r="Q93" s="10">
-        <v>1685</v>
+        <v>0</v>
       </c>
       <c r="R93" s="10">
-        <v>1575</v>
+        <v>0</v>
       </c>
       <c r="S93" s="10">
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="T93" s="10">
-        <v>1820</v>
+        <v>0</v>
       </c>
       <c r="U93" s="10">
-        <v>1885</v>
-      </c>
-      <c r="V93" s="5"/>
-      <c r="W93" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="V93" s="10">
+        <v>0</v>
+      </c>
+      <c r="W93" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
@@ -7314,64 +7330,64 @@
         <v>69</v>
       </c>
       <c r="D94" s="10">
-        <v>440</v>
+        <v>0</v>
       </c>
       <c r="E94" s="10">
-        <v>600</v>
-      </c>
-      <c r="F94" s="5">
-        <v>595</v>
+        <v>0</v>
+      </c>
+      <c r="F94" s="10">
+        <v>0</v>
       </c>
       <c r="G94" s="10">
-        <v>715</v>
+        <v>0</v>
       </c>
       <c r="H94" s="10">
-        <v>885</v>
+        <v>0</v>
       </c>
       <c r="I94" s="10">
-        <v>1065</v>
+        <v>0</v>
       </c>
       <c r="J94" s="10">
-        <v>1205</v>
+        <v>0</v>
       </c>
       <c r="K94" s="10">
-        <v>1355</v>
+        <v>0</v>
       </c>
       <c r="L94" s="10">
-        <v>1495</v>
+        <v>0</v>
       </c>
       <c r="M94" s="10">
-        <v>1640</v>
+        <v>0</v>
       </c>
       <c r="N94" s="10">
-        <v>1750</v>
+        <v>0</v>
       </c>
       <c r="O94" s="10">
-        <v>1865</v>
+        <v>0</v>
       </c>
       <c r="P94" s="10">
-        <v>1975</v>
+        <v>0</v>
       </c>
       <c r="Q94" s="10">
-        <v>2090</v>
+        <v>0</v>
       </c>
       <c r="R94" s="10">
-        <v>2195</v>
+        <v>0</v>
       </c>
       <c r="S94" s="10">
-        <v>2310</v>
+        <v>0</v>
       </c>
       <c r="T94" s="10">
-        <v>2415</v>
+        <v>0</v>
       </c>
       <c r="U94" s="10">
-        <v>2530</v>
+        <v>0</v>
       </c>
       <c r="V94" s="10">
-        <v>2645</v>
+        <v>0</v>
       </c>
       <c r="W94" s="10">
-        <v>2760</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:23" x14ac:dyDescent="0.25">
@@ -7385,64 +7401,64 @@
         <v>69</v>
       </c>
       <c r="D95" s="10">
-        <v>405</v>
+        <v>0</v>
       </c>
       <c r="E95" s="10">
-        <v>760</v>
-      </c>
-      <c r="F95" s="5">
-        <v>1140</v>
+        <v>0</v>
+      </c>
+      <c r="F95" s="10">
+        <v>0</v>
       </c>
       <c r="G95" s="10">
-        <v>1135</v>
+        <v>0</v>
       </c>
       <c r="H95" s="10">
-        <v>1205</v>
+        <v>0</v>
       </c>
       <c r="I95" s="10">
-        <v>1340</v>
+        <v>0</v>
       </c>
       <c r="J95" s="10">
-        <v>1600</v>
+        <v>0</v>
       </c>
       <c r="K95" s="10">
-        <v>1595</v>
+        <v>0</v>
       </c>
       <c r="L95" s="10">
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="M95" s="10">
-        <v>1935</v>
+        <v>0</v>
       </c>
       <c r="N95" s="10">
-        <v>1925</v>
+        <v>0</v>
       </c>
       <c r="O95" s="10">
-        <v>2030</v>
+        <v>0</v>
       </c>
       <c r="P95" s="10">
-        <v>2225</v>
+        <v>0</v>
       </c>
       <c r="Q95" s="10">
-        <v>2425</v>
+        <v>0</v>
       </c>
       <c r="R95" s="10">
-        <v>2260</v>
+        <v>0</v>
       </c>
       <c r="S95" s="10">
-        <v>2445</v>
+        <v>0</v>
       </c>
       <c r="T95" s="10">
-        <v>2615</v>
+        <v>0</v>
       </c>
       <c r="U95" s="10">
-        <v>2705</v>
+        <v>0</v>
       </c>
       <c r="V95" s="10">
-        <v>2795</v>
+        <v>0</v>
       </c>
       <c r="W95" s="10">
-        <v>2890</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:23" x14ac:dyDescent="0.25">
@@ -7456,31 +7472,65 @@
         <v>69</v>
       </c>
       <c r="D96" s="10">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="E96" s="10">
-        <v>845</v>
-      </c>
-      <c r="F96" s="5">
-        <v>1270</v>
-      </c>
-      <c r="G96" s="5"/>
-      <c r="H96" s="5"/>
-      <c r="I96" s="5"/>
-      <c r="J96" s="5"/>
-      <c r="K96" s="5"/>
-      <c r="L96" s="5"/>
-      <c r="M96" s="5"/>
-      <c r="N96" s="5"/>
-      <c r="O96" s="5"/>
-      <c r="P96" s="5"/>
-      <c r="Q96" s="5"/>
-      <c r="R96" s="5"/>
-      <c r="S96" s="5"/>
-      <c r="T96" s="5"/>
-      <c r="U96" s="5"/>
-      <c r="V96" s="5"/>
-      <c r="W96" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="F96" s="10">
+        <v>0</v>
+      </c>
+      <c r="G96" s="10">
+        <v>0</v>
+      </c>
+      <c r="H96" s="10">
+        <v>0</v>
+      </c>
+      <c r="I96" s="10">
+        <v>0</v>
+      </c>
+      <c r="J96" s="10">
+        <v>0</v>
+      </c>
+      <c r="K96" s="10">
+        <v>0</v>
+      </c>
+      <c r="L96" s="10">
+        <v>0</v>
+      </c>
+      <c r="M96" s="10">
+        <v>0</v>
+      </c>
+      <c r="N96" s="10">
+        <v>0</v>
+      </c>
+      <c r="O96" s="10">
+        <v>0</v>
+      </c>
+      <c r="P96" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q96" s="10">
+        <v>0</v>
+      </c>
+      <c r="R96" s="10">
+        <v>0</v>
+      </c>
+      <c r="S96" s="10">
+        <v>0</v>
+      </c>
+      <c r="T96" s="10">
+        <v>0</v>
+      </c>
+      <c r="U96" s="10">
+        <v>0</v>
+      </c>
+      <c r="V96" s="10">
+        <v>0</v>
+      </c>
+      <c r="W96" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
@@ -7493,64 +7543,64 @@
         <v>69</v>
       </c>
       <c r="D97" s="10">
-        <v>355</v>
+        <v>0</v>
       </c>
       <c r="E97" s="10">
-        <v>660</v>
-      </c>
-      <c r="F97" s="5">
-        <v>995</v>
+        <v>0</v>
+      </c>
+      <c r="F97" s="10">
+        <v>0</v>
       </c>
       <c r="G97" s="10">
-        <v>1075</v>
+        <v>0</v>
       </c>
       <c r="H97" s="10">
-        <v>1160</v>
+        <v>0</v>
       </c>
       <c r="I97" s="10">
-        <v>1290</v>
+        <v>0</v>
       </c>
       <c r="J97" s="10">
-        <v>1530</v>
+        <v>0</v>
       </c>
       <c r="K97" s="10">
-        <v>1560</v>
+        <v>0</v>
       </c>
       <c r="L97" s="10">
-        <v>1665</v>
+        <v>0</v>
       </c>
       <c r="M97" s="10">
-        <v>1885</v>
+        <v>0</v>
       </c>
       <c r="N97" s="10">
-        <v>1900</v>
+        <v>0</v>
       </c>
       <c r="O97" s="10">
-        <v>2005</v>
+        <v>0</v>
       </c>
       <c r="P97" s="10">
-        <v>2185</v>
+        <v>0</v>
       </c>
       <c r="Q97" s="10">
-        <v>2390</v>
+        <v>0</v>
       </c>
       <c r="R97" s="10">
-        <v>2230</v>
+        <v>0</v>
       </c>
       <c r="S97" s="10">
-        <v>2410</v>
+        <v>0</v>
       </c>
       <c r="T97" s="10">
-        <v>2580</v>
+        <v>0</v>
       </c>
       <c r="U97" s="10">
-        <v>2755</v>
+        <v>0</v>
       </c>
       <c r="V97" s="10">
-        <v>2935</v>
+        <v>0</v>
       </c>
       <c r="W97" s="10">
-        <v>3115</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:23" x14ac:dyDescent="0.25">
@@ -7564,31 +7614,65 @@
         <v>69</v>
       </c>
       <c r="D98" s="10">
-        <v>460</v>
+        <v>0</v>
       </c>
       <c r="E98" s="10">
-        <v>835</v>
-      </c>
-      <c r="F98" s="5">
-        <v>1260</v>
-      </c>
-      <c r="G98" s="5"/>
-      <c r="H98" s="5"/>
-      <c r="I98" s="5"/>
-      <c r="J98" s="5"/>
-      <c r="K98" s="5"/>
-      <c r="L98" s="5"/>
-      <c r="M98" s="5"/>
-      <c r="N98" s="5"/>
-      <c r="O98" s="5"/>
-      <c r="P98" s="5"/>
-      <c r="Q98" s="5"/>
-      <c r="R98" s="5"/>
-      <c r="S98" s="5"/>
-      <c r="T98" s="5"/>
-      <c r="U98" s="5"/>
-      <c r="V98" s="5"/>
-      <c r="W98" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="F98" s="10">
+        <v>0</v>
+      </c>
+      <c r="G98" s="10">
+        <v>0</v>
+      </c>
+      <c r="H98" s="10">
+        <v>0</v>
+      </c>
+      <c r="I98" s="10">
+        <v>0</v>
+      </c>
+      <c r="J98" s="10">
+        <v>0</v>
+      </c>
+      <c r="K98" s="10">
+        <v>0</v>
+      </c>
+      <c r="L98" s="10">
+        <v>0</v>
+      </c>
+      <c r="M98" s="10">
+        <v>0</v>
+      </c>
+      <c r="N98" s="10">
+        <v>0</v>
+      </c>
+      <c r="O98" s="10">
+        <v>0</v>
+      </c>
+      <c r="P98" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q98" s="10">
+        <v>0</v>
+      </c>
+      <c r="R98" s="10">
+        <v>0</v>
+      </c>
+      <c r="S98" s="10">
+        <v>0</v>
+      </c>
+      <c r="T98" s="10">
+        <v>0</v>
+      </c>
+      <c r="U98" s="10">
+        <v>0</v>
+      </c>
+      <c r="V98" s="10">
+        <v>0</v>
+      </c>
+      <c r="W98" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
@@ -7601,31 +7685,65 @@
         <v>69</v>
       </c>
       <c r="D99" s="10">
-        <v>370</v>
+        <v>0</v>
       </c>
       <c r="E99" s="10">
-        <v>665</v>
-      </c>
-      <c r="F99" s="5">
-        <v>1005</v>
-      </c>
-      <c r="G99" s="5"/>
-      <c r="H99" s="5"/>
-      <c r="I99" s="5"/>
-      <c r="J99" s="5"/>
-      <c r="K99" s="5"/>
-      <c r="L99" s="5"/>
-      <c r="M99" s="5"/>
-      <c r="N99" s="5"/>
-      <c r="O99" s="5"/>
-      <c r="P99" s="5"/>
-      <c r="Q99" s="5"/>
-      <c r="R99" s="5"/>
-      <c r="S99" s="5"/>
-      <c r="T99" s="5"/>
-      <c r="U99" s="5"/>
-      <c r="V99" s="5"/>
-      <c r="W99" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="F99" s="10">
+        <v>0</v>
+      </c>
+      <c r="G99" s="10">
+        <v>0</v>
+      </c>
+      <c r="H99" s="10">
+        <v>0</v>
+      </c>
+      <c r="I99" s="10">
+        <v>0</v>
+      </c>
+      <c r="J99" s="10">
+        <v>0</v>
+      </c>
+      <c r="K99" s="10">
+        <v>0</v>
+      </c>
+      <c r="L99" s="10">
+        <v>0</v>
+      </c>
+      <c r="M99" s="10">
+        <v>0</v>
+      </c>
+      <c r="N99" s="10">
+        <v>0</v>
+      </c>
+      <c r="O99" s="10">
+        <v>0</v>
+      </c>
+      <c r="P99" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q99" s="10">
+        <v>0</v>
+      </c>
+      <c r="R99" s="10">
+        <v>0</v>
+      </c>
+      <c r="S99" s="10">
+        <v>0</v>
+      </c>
+      <c r="T99" s="10">
+        <v>0</v>
+      </c>
+      <c r="U99" s="10">
+        <v>0</v>
+      </c>
+      <c r="V99" s="10">
+        <v>0</v>
+      </c>
+      <c r="W99" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
@@ -7638,31 +7756,65 @@
         <v>69</v>
       </c>
       <c r="D100" s="10">
-        <v>355</v>
+        <v>0</v>
       </c>
       <c r="E100" s="10">
-        <v>645</v>
-      </c>
-      <c r="F100" s="5">
-        <v>975</v>
-      </c>
-      <c r="G100" s="5"/>
-      <c r="H100" s="5"/>
-      <c r="I100" s="5"/>
-      <c r="J100" s="5"/>
-      <c r="K100" s="5"/>
-      <c r="L100" s="5"/>
-      <c r="M100" s="5"/>
-      <c r="N100" s="5"/>
-      <c r="O100" s="5"/>
-      <c r="P100" s="5"/>
-      <c r="Q100" s="5"/>
-      <c r="R100" s="5"/>
-      <c r="S100" s="5"/>
-      <c r="T100" s="5"/>
-      <c r="U100" s="5"/>
-      <c r="V100" s="5"/>
-      <c r="W100" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="F100" s="10">
+        <v>0</v>
+      </c>
+      <c r="G100" s="10">
+        <v>0</v>
+      </c>
+      <c r="H100" s="10">
+        <v>0</v>
+      </c>
+      <c r="I100" s="10">
+        <v>0</v>
+      </c>
+      <c r="J100" s="10">
+        <v>0</v>
+      </c>
+      <c r="K100" s="10">
+        <v>0</v>
+      </c>
+      <c r="L100" s="10">
+        <v>0</v>
+      </c>
+      <c r="M100" s="10">
+        <v>0</v>
+      </c>
+      <c r="N100" s="10">
+        <v>0</v>
+      </c>
+      <c r="O100" s="10">
+        <v>0</v>
+      </c>
+      <c r="P100" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q100" s="10">
+        <v>0</v>
+      </c>
+      <c r="R100" s="10">
+        <v>0</v>
+      </c>
+      <c r="S100" s="10">
+        <v>0</v>
+      </c>
+      <c r="T100" s="10">
+        <v>0</v>
+      </c>
+      <c r="U100" s="10">
+        <v>0</v>
+      </c>
+      <c r="V100" s="10">
+        <v>0</v>
+      </c>
+      <c r="W100" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
@@ -7675,31 +7827,65 @@
         <v>69</v>
       </c>
       <c r="D101" s="10">
-        <v>370</v>
+        <v>0</v>
       </c>
       <c r="E101" s="10">
-        <v>665</v>
-      </c>
-      <c r="F101" s="5">
-        <v>1005</v>
-      </c>
-      <c r="G101" s="5"/>
-      <c r="H101" s="5"/>
-      <c r="I101" s="5"/>
-      <c r="J101" s="5"/>
-      <c r="K101" s="5"/>
-      <c r="L101" s="5"/>
-      <c r="M101" s="5"/>
-      <c r="N101" s="5"/>
-      <c r="O101" s="5"/>
-      <c r="P101" s="5"/>
-      <c r="Q101" s="5"/>
-      <c r="R101" s="5"/>
-      <c r="S101" s="5"/>
-      <c r="T101" s="5"/>
-      <c r="U101" s="5"/>
-      <c r="V101" s="5"/>
-      <c r="W101" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="F101" s="10">
+        <v>0</v>
+      </c>
+      <c r="G101" s="10">
+        <v>0</v>
+      </c>
+      <c r="H101" s="10">
+        <v>0</v>
+      </c>
+      <c r="I101" s="10">
+        <v>0</v>
+      </c>
+      <c r="J101" s="10">
+        <v>0</v>
+      </c>
+      <c r="K101" s="10">
+        <v>0</v>
+      </c>
+      <c r="L101" s="10">
+        <v>0</v>
+      </c>
+      <c r="M101" s="10">
+        <v>0</v>
+      </c>
+      <c r="N101" s="10">
+        <v>0</v>
+      </c>
+      <c r="O101" s="10">
+        <v>0</v>
+      </c>
+      <c r="P101" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q101" s="10">
+        <v>0</v>
+      </c>
+      <c r="R101" s="10">
+        <v>0</v>
+      </c>
+      <c r="S101" s="10">
+        <v>0</v>
+      </c>
+      <c r="T101" s="10">
+        <v>0</v>
+      </c>
+      <c r="U101" s="10">
+        <v>0</v>
+      </c>
+      <c r="V101" s="10">
+        <v>0</v>
+      </c>
+      <c r="W101" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
@@ -7712,31 +7898,65 @@
         <v>69</v>
       </c>
       <c r="D102" s="10">
-        <v>360</v>
+        <v>0</v>
       </c>
       <c r="E102" s="10">
-        <v>650</v>
-      </c>
-      <c r="F102" s="5">
-        <v>980</v>
-      </c>
-      <c r="G102" s="5"/>
-      <c r="H102" s="5"/>
-      <c r="I102" s="5"/>
-      <c r="J102" s="5"/>
-      <c r="K102" s="5"/>
-      <c r="L102" s="5"/>
-      <c r="M102" s="5"/>
-      <c r="N102" s="5"/>
-      <c r="O102" s="5"/>
-      <c r="P102" s="5"/>
-      <c r="Q102" s="5"/>
-      <c r="R102" s="5"/>
-      <c r="S102" s="5"/>
-      <c r="T102" s="5"/>
-      <c r="U102" s="5"/>
-      <c r="V102" s="5"/>
-      <c r="W102" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="F102" s="10">
+        <v>0</v>
+      </c>
+      <c r="G102" s="10">
+        <v>0</v>
+      </c>
+      <c r="H102" s="10">
+        <v>0</v>
+      </c>
+      <c r="I102" s="10">
+        <v>0</v>
+      </c>
+      <c r="J102" s="10">
+        <v>0</v>
+      </c>
+      <c r="K102" s="10">
+        <v>0</v>
+      </c>
+      <c r="L102" s="10">
+        <v>0</v>
+      </c>
+      <c r="M102" s="10">
+        <v>0</v>
+      </c>
+      <c r="N102" s="10">
+        <v>0</v>
+      </c>
+      <c r="O102" s="10">
+        <v>0</v>
+      </c>
+      <c r="P102" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q102" s="10">
+        <v>0</v>
+      </c>
+      <c r="R102" s="10">
+        <v>0</v>
+      </c>
+      <c r="S102" s="10">
+        <v>0</v>
+      </c>
+      <c r="T102" s="10">
+        <v>0</v>
+      </c>
+      <c r="U102" s="10">
+        <v>0</v>
+      </c>
+      <c r="V102" s="10">
+        <v>0</v>
+      </c>
+      <c r="W102" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
@@ -7749,31 +7969,65 @@
         <v>69</v>
       </c>
       <c r="D103" s="10">
-        <v>340</v>
+        <v>0</v>
       </c>
       <c r="E103" s="10">
-        <v>640</v>
-      </c>
-      <c r="F103" s="5">
-        <v>955</v>
-      </c>
-      <c r="G103" s="5"/>
-      <c r="H103" s="5"/>
-      <c r="I103" s="5"/>
-      <c r="J103" s="5"/>
-      <c r="K103" s="5"/>
-      <c r="L103" s="5"/>
-      <c r="M103" s="5"/>
-      <c r="N103" s="5"/>
-      <c r="O103" s="5"/>
-      <c r="P103" s="5"/>
-      <c r="Q103" s="5"/>
-      <c r="R103" s="5"/>
-      <c r="S103" s="5"/>
-      <c r="T103" s="5"/>
-      <c r="U103" s="5"/>
-      <c r="V103" s="5"/>
-      <c r="W103" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="F103" s="10">
+        <v>0</v>
+      </c>
+      <c r="G103" s="10">
+        <v>0</v>
+      </c>
+      <c r="H103" s="10">
+        <v>0</v>
+      </c>
+      <c r="I103" s="10">
+        <v>0</v>
+      </c>
+      <c r="J103" s="10">
+        <v>0</v>
+      </c>
+      <c r="K103" s="10">
+        <v>0</v>
+      </c>
+      <c r="L103" s="10">
+        <v>0</v>
+      </c>
+      <c r="M103" s="10">
+        <v>0</v>
+      </c>
+      <c r="N103" s="10">
+        <v>0</v>
+      </c>
+      <c r="O103" s="10">
+        <v>0</v>
+      </c>
+      <c r="P103" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q103" s="10">
+        <v>0</v>
+      </c>
+      <c r="R103" s="10">
+        <v>0</v>
+      </c>
+      <c r="S103" s="10">
+        <v>0</v>
+      </c>
+      <c r="T103" s="10">
+        <v>0</v>
+      </c>
+      <c r="U103" s="10">
+        <v>0</v>
+      </c>
+      <c r="V103" s="10">
+        <v>0</v>
+      </c>
+      <c r="W103" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
@@ -7786,31 +8040,65 @@
         <v>69</v>
       </c>
       <c r="D104" s="10">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="E104" s="10">
-        <v>695</v>
-      </c>
-      <c r="F104" s="5">
-        <v>1040</v>
-      </c>
-      <c r="G104" s="5"/>
-      <c r="H104" s="5"/>
-      <c r="I104" s="5"/>
-      <c r="J104" s="5"/>
-      <c r="K104" s="5"/>
-      <c r="L104" s="5"/>
-      <c r="M104" s="5"/>
-      <c r="N104" s="5"/>
-      <c r="O104" s="5"/>
-      <c r="P104" s="5"/>
-      <c r="Q104" s="5"/>
-      <c r="R104" s="5"/>
-      <c r="S104" s="5"/>
-      <c r="T104" s="5"/>
-      <c r="U104" s="5"/>
-      <c r="V104" s="5"/>
-      <c r="W104" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="F104" s="10">
+        <v>0</v>
+      </c>
+      <c r="G104" s="10">
+        <v>0</v>
+      </c>
+      <c r="H104" s="10">
+        <v>0</v>
+      </c>
+      <c r="I104" s="10">
+        <v>0</v>
+      </c>
+      <c r="J104" s="10">
+        <v>0</v>
+      </c>
+      <c r="K104" s="10">
+        <v>0</v>
+      </c>
+      <c r="L104" s="10">
+        <v>0</v>
+      </c>
+      <c r="M104" s="10">
+        <v>0</v>
+      </c>
+      <c r="N104" s="10">
+        <v>0</v>
+      </c>
+      <c r="O104" s="10">
+        <v>0</v>
+      </c>
+      <c r="P104" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q104" s="10">
+        <v>0</v>
+      </c>
+      <c r="R104" s="10">
+        <v>0</v>
+      </c>
+      <c r="S104" s="10">
+        <v>0</v>
+      </c>
+      <c r="T104" s="10">
+        <v>0</v>
+      </c>
+      <c r="U104" s="10">
+        <v>0</v>
+      </c>
+      <c r="V104" s="10">
+        <v>0</v>
+      </c>
+      <c r="W104" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
@@ -7823,31 +8111,65 @@
         <v>69</v>
       </c>
       <c r="D105" s="10">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="E105" s="10">
-        <v>405</v>
-      </c>
-      <c r="F105" s="5">
-        <v>600</v>
-      </c>
-      <c r="G105" s="5"/>
-      <c r="H105" s="5"/>
-      <c r="I105" s="5"/>
-      <c r="J105" s="5"/>
-      <c r="K105" s="5"/>
-      <c r="L105" s="5"/>
-      <c r="M105" s="5"/>
-      <c r="N105" s="5"/>
-      <c r="O105" s="5"/>
-      <c r="P105" s="5"/>
-      <c r="Q105" s="5"/>
-      <c r="R105" s="5"/>
-      <c r="S105" s="5"/>
-      <c r="T105" s="5"/>
-      <c r="U105" s="5"/>
-      <c r="V105" s="5"/>
-      <c r="W105" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="F105" s="10">
+        <v>0</v>
+      </c>
+      <c r="G105" s="10">
+        <v>0</v>
+      </c>
+      <c r="H105" s="10">
+        <v>0</v>
+      </c>
+      <c r="I105" s="10">
+        <v>0</v>
+      </c>
+      <c r="J105" s="10">
+        <v>0</v>
+      </c>
+      <c r="K105" s="10">
+        <v>0</v>
+      </c>
+      <c r="L105" s="10">
+        <v>0</v>
+      </c>
+      <c r="M105" s="10">
+        <v>0</v>
+      </c>
+      <c r="N105" s="10">
+        <v>0</v>
+      </c>
+      <c r="O105" s="10">
+        <v>0</v>
+      </c>
+      <c r="P105" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q105" s="10">
+        <v>0</v>
+      </c>
+      <c r="R105" s="10">
+        <v>0</v>
+      </c>
+      <c r="S105" s="10">
+        <v>0</v>
+      </c>
+      <c r="T105" s="10">
+        <v>0</v>
+      </c>
+      <c r="U105" s="10">
+        <v>0</v>
+      </c>
+      <c r="V105" s="10">
+        <v>0</v>
+      </c>
+      <c r="W105" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
@@ -7860,31 +8182,65 @@
         <v>69</v>
       </c>
       <c r="D106" s="10">
-        <v>435</v>
+        <v>0</v>
       </c>
       <c r="E106" s="10">
-        <v>825</v>
-      </c>
-      <c r="F106" s="5">
-        <v>1240</v>
-      </c>
-      <c r="G106" s="5"/>
-      <c r="H106" s="5"/>
-      <c r="I106" s="5"/>
-      <c r="J106" s="5"/>
-      <c r="K106" s="5"/>
-      <c r="L106" s="5"/>
-      <c r="M106" s="5"/>
-      <c r="N106" s="5"/>
-      <c r="O106" s="5"/>
-      <c r="P106" s="5"/>
-      <c r="Q106" s="5"/>
-      <c r="R106" s="5"/>
-      <c r="S106" s="5"/>
-      <c r="T106" s="5"/>
-      <c r="U106" s="5"/>
-      <c r="V106" s="5"/>
-      <c r="W106" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="F106" s="10">
+        <v>0</v>
+      </c>
+      <c r="G106" s="10">
+        <v>0</v>
+      </c>
+      <c r="H106" s="10">
+        <v>0</v>
+      </c>
+      <c r="I106" s="10">
+        <v>0</v>
+      </c>
+      <c r="J106" s="10">
+        <v>0</v>
+      </c>
+      <c r="K106" s="10">
+        <v>0</v>
+      </c>
+      <c r="L106" s="10">
+        <v>0</v>
+      </c>
+      <c r="M106" s="10">
+        <v>0</v>
+      </c>
+      <c r="N106" s="10">
+        <v>0</v>
+      </c>
+      <c r="O106" s="10">
+        <v>0</v>
+      </c>
+      <c r="P106" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q106" s="10">
+        <v>0</v>
+      </c>
+      <c r="R106" s="10">
+        <v>0</v>
+      </c>
+      <c r="S106" s="10">
+        <v>0</v>
+      </c>
+      <c r="T106" s="10">
+        <v>0</v>
+      </c>
+      <c r="U106" s="10">
+        <v>0</v>
+      </c>
+      <c r="V106" s="10">
+        <v>0</v>
+      </c>
+      <c r="W106" s="10">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add out of range plt qty & cities + excp handlers
</commit_message>
<xml_diff>
--- a/db/passport.xlsx
+++ b/db/passport.xlsx
@@ -729,9 +729,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W111"/>
+  <dimension ref="A1:AG111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L16" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -741,7 +743,7 @@
     <col min="24" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -811,8 +813,38 @@
       <c r="W1" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="3">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="3">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="3">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="3">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="3">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="3">
+        <v>27</v>
+      </c>
+      <c r="AE1" s="3">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="3">
+        <v>29</v>
+      </c>
+      <c r="AG1" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -883,7 +915,7 @@
         <v>4240</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -954,7 +986,7 @@
         <v>4240</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1025,7 +1057,7 @@
         <v>4860</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -1096,7 +1128,7 @@
         <v>4365</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
@@ -1167,7 +1199,7 @@
         <v>4365</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>0</v>
       </c>
@@ -1238,7 +1270,7 @@
         <v>3865</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>0</v>
       </c>
@@ -1309,7 +1341,7 @@
         <v>8600</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
@@ -1380,7 +1412,7 @@
         <v>8850</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>0</v>
       </c>
@@ -1451,7 +1483,7 @@
         <v>7605</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>0</v>
       </c>
@@ -1522,7 +1554,7 @@
         <v>5735</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>0</v>
       </c>
@@ -1593,7 +1625,7 @@
         <v>6980</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
@@ -1664,7 +1696,7 @@
         <v>6480</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>0</v>
       </c>
@@ -1735,7 +1767,7 @@
         <v>5805</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>0</v>
       </c>
@@ -1806,7 +1838,7 @@
         <v>7105</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>0</v>
       </c>
@@ -1877,7 +1909,7 @@
         <v>5180</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>0</v>
       </c>
@@ -1948,7 +1980,7 @@
         <v>5235</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>0</v>
       </c>
@@ -2019,7 +2051,7 @@
         <v>4115</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>0</v>
       </c>
@@ -2090,7 +2122,7 @@
         <v>4365</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>0</v>
       </c>
@@ -2161,7 +2193,7 @@
         <v>8350</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>0</v>
       </c>
@@ -2232,7 +2264,7 @@
         <v>6870</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>0</v>
       </c>
@@ -2303,7 +2335,7 @@
         <v>5985</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>0</v>
       </c>
@@ -2374,7 +2406,7 @@
         <v>5395</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>0</v>
       </c>
@@ -2445,7 +2477,7 @@
         <v>3115</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>0</v>
       </c>
@@ -2516,7 +2548,7 @@
         <v>4545</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>0</v>
       </c>
@@ -2587,7 +2619,7 @@
         <v>6730</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>1</v>
       </c>
@@ -2658,7 +2690,7 @@
         <v>6635</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>1</v>
       </c>
@@ -2729,7 +2761,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>1</v>
       </c>
@@ -2800,7 +2832,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>1</v>
       </c>
@@ -2870,8 +2902,38 @@
       <c r="W30" s="4">
         <v>430</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X30" s="4">
+        <v>430</v>
+      </c>
+      <c r="Y30" s="4">
+        <v>430</v>
+      </c>
+      <c r="Z30" s="4">
+        <v>430</v>
+      </c>
+      <c r="AA30" s="4">
+        <v>430</v>
+      </c>
+      <c r="AB30" s="4">
+        <v>430</v>
+      </c>
+      <c r="AC30" s="4">
+        <v>430</v>
+      </c>
+      <c r="AD30" s="4">
+        <v>430</v>
+      </c>
+      <c r="AE30" s="4">
+        <v>430</v>
+      </c>
+      <c r="AF30" s="4">
+        <v>430</v>
+      </c>
+      <c r="AG30" s="4">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>1</v>
       </c>
@@ -2942,7 +3004,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
add orlando, 21-30 for tracy
</commit_message>
<xml_diff>
--- a/db/passport.xlsx
+++ b/db/passport.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$V$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$V$73</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="80">
   <si>
     <t>Kent, WA</t>
   </si>
@@ -726,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG108"/>
+  <dimension ref="A1:AG109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B48" sqref="A48:XFD48"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2686,6 +2686,36 @@
       <c r="W27" s="4">
         <v>1400</v>
       </c>
+      <c r="X27" s="4">
+        <v>1400</v>
+      </c>
+      <c r="Y27" s="4">
+        <v>1400</v>
+      </c>
+      <c r="Z27" s="4">
+        <v>1400</v>
+      </c>
+      <c r="AA27" s="4">
+        <v>1400</v>
+      </c>
+      <c r="AB27" s="4">
+        <v>1400</v>
+      </c>
+      <c r="AC27" s="4">
+        <v>1400</v>
+      </c>
+      <c r="AD27" s="4">
+        <v>1400</v>
+      </c>
+      <c r="AE27" s="4">
+        <v>1400</v>
+      </c>
+      <c r="AF27" s="4">
+        <v>1400</v>
+      </c>
+      <c r="AG27" s="4">
+        <v>1400</v>
+      </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
@@ -3431,71 +3461,71 @@
       <c r="A38" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>42</v>
+      <c r="B38" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="4">
-        <v>630</v>
+        <v>690</v>
       </c>
       <c r="E38" s="4">
-        <v>1070</v>
+        <v>990</v>
       </c>
       <c r="F38" s="4">
-        <v>1495</v>
+        <v>1395</v>
       </c>
       <c r="G38" s="4">
-        <v>1930</v>
+        <v>1840</v>
       </c>
       <c r="H38" s="4">
-        <v>2260</v>
+        <v>2285</v>
       </c>
       <c r="I38" s="4">
-        <v>2870</v>
+        <v>2720</v>
       </c>
       <c r="J38" s="4">
-        <v>3015</v>
+        <v>3160</v>
       </c>
       <c r="K38" s="4">
-        <v>3205</v>
+        <v>3580</v>
       </c>
       <c r="L38" s="4">
-        <v>3560</v>
+        <v>3950</v>
       </c>
       <c r="M38" s="4">
-        <v>3850</v>
+        <v>4270</v>
       </c>
       <c r="N38" s="4">
-        <v>4213</v>
+        <v>4605</v>
       </c>
       <c r="O38" s="4">
-        <v>4572</v>
+        <v>4975</v>
       </c>
       <c r="P38" s="4">
-        <v>4927</v>
+        <v>5330</v>
       </c>
       <c r="Q38" s="4">
-        <v>5278</v>
+        <v>5680</v>
       </c>
       <c r="R38" s="4">
-        <v>5625</v>
+        <v>6025</v>
       </c>
       <c r="S38" s="4">
-        <v>5968</v>
+        <v>6355</v>
       </c>
       <c r="T38" s="4">
-        <v>6307</v>
+        <v>6680</v>
       </c>
       <c r="U38" s="4">
-        <v>6642</v>
+        <v>6995</v>
       </c>
       <c r="V38" s="4">
-        <v>6973</v>
+        <v>7305</v>
       </c>
       <c r="W38" s="4">
-        <v>7300</v>
+        <v>7550</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -3503,7 +3533,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>6</v>
@@ -3574,7 +3604,7 @@
         <v>1</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>6</v>
@@ -3645,70 +3675,70 @@
         <v>1</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="4">
-        <v>520</v>
+        <v>630</v>
       </c>
       <c r="E41" s="4">
-        <v>1010</v>
+        <v>1070</v>
       </c>
       <c r="F41" s="4">
-        <v>1445</v>
+        <v>1495</v>
       </c>
       <c r="G41" s="4">
-        <v>1865</v>
+        <v>1930</v>
       </c>
       <c r="H41" s="4">
-        <v>2200</v>
+        <v>2260</v>
       </c>
       <c r="I41" s="4">
-        <v>2585</v>
+        <v>2870</v>
       </c>
       <c r="J41" s="4">
-        <v>2920</v>
+        <v>3015</v>
       </c>
       <c r="K41" s="4">
-        <v>3245</v>
+        <v>3205</v>
       </c>
       <c r="L41" s="4">
-        <v>3370</v>
+        <v>3560</v>
       </c>
       <c r="M41" s="4">
-        <v>3640</v>
+        <v>3850</v>
       </c>
       <c r="N41" s="4">
-        <v>3925</v>
+        <v>4213</v>
       </c>
       <c r="O41" s="4">
-        <v>4240</v>
+        <v>4572</v>
       </c>
       <c r="P41" s="4">
-        <v>4545</v>
+        <v>4927</v>
       </c>
       <c r="Q41" s="4">
-        <v>4845</v>
+        <v>5278</v>
       </c>
       <c r="R41" s="4">
-        <v>5135</v>
+        <v>5625</v>
       </c>
       <c r="S41" s="4">
-        <v>5420</v>
+        <v>5968</v>
       </c>
       <c r="T41" s="4">
-        <v>5695</v>
+        <v>6307</v>
       </c>
       <c r="U41" s="4">
-        <v>6030</v>
+        <v>6642</v>
       </c>
       <c r="V41" s="4">
-        <v>6365</v>
+        <v>6973</v>
       </c>
       <c r="W41" s="4">
-        <v>6700</v>
+        <v>7300</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
@@ -3716,16 +3746,16 @@
         <v>1</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="4">
-        <v>575</v>
+        <v>520</v>
       </c>
       <c r="E42" s="4">
-        <v>1040</v>
+        <v>1010</v>
       </c>
       <c r="F42" s="4">
         <v>1445</v>
@@ -3740,46 +3770,46 @@
         <v>2585</v>
       </c>
       <c r="J42" s="4">
-        <v>2685</v>
+        <v>2920</v>
       </c>
       <c r="K42" s="4">
-        <v>3120</v>
+        <v>3245</v>
       </c>
       <c r="L42" s="4">
-        <v>3280</v>
+        <v>3370</v>
       </c>
       <c r="M42" s="4">
-        <v>3435</v>
+        <v>3640</v>
       </c>
       <c r="N42" s="4">
-        <v>3705</v>
+        <v>3925</v>
       </c>
       <c r="O42" s="4">
-        <v>4000</v>
+        <v>4240</v>
       </c>
       <c r="P42" s="4">
-        <v>4290</v>
+        <v>4545</v>
       </c>
       <c r="Q42" s="4">
-        <v>4570</v>
+        <v>4845</v>
       </c>
       <c r="R42" s="4">
-        <v>4845</v>
+        <v>5135</v>
       </c>
       <c r="S42" s="4">
-        <v>5115</v>
+        <v>5420</v>
       </c>
       <c r="T42" s="4">
-        <v>5375</v>
+        <v>5695</v>
       </c>
       <c r="U42" s="4">
-        <v>5690</v>
+        <v>6030</v>
       </c>
       <c r="V42" s="4">
-        <v>6005</v>
+        <v>6365</v>
       </c>
       <c r="W42" s="4">
-        <v>6325</v>
+        <v>6700</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
@@ -3787,70 +3817,70 @@
         <v>1</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="4">
-        <v>475</v>
+        <v>575</v>
       </c>
       <c r="E43" s="4">
-        <v>860</v>
+        <v>1040</v>
       </c>
       <c r="F43" s="4">
-        <v>1265</v>
+        <v>1445</v>
       </c>
       <c r="G43" s="4">
-        <v>1630</v>
+        <v>1865</v>
       </c>
       <c r="H43" s="4">
-        <v>1965</v>
+        <v>2200</v>
       </c>
       <c r="I43" s="4">
-        <v>2310</v>
+        <v>2585</v>
       </c>
       <c r="J43" s="4">
-        <v>2620</v>
+        <v>2685</v>
       </c>
       <c r="K43" s="4">
-        <v>2955</v>
+        <v>3120</v>
       </c>
       <c r="L43" s="4">
-        <v>3140</v>
+        <v>3280</v>
       </c>
       <c r="M43" s="4">
-        <v>3280</v>
+        <v>3435</v>
       </c>
       <c r="N43" s="4">
-        <v>3540</v>
+        <v>3705</v>
       </c>
       <c r="O43" s="4">
-        <v>3820</v>
+        <v>4000</v>
       </c>
       <c r="P43" s="4">
-        <v>4095</v>
+        <v>4290</v>
       </c>
       <c r="Q43" s="4">
-        <v>4365</v>
+        <v>4570</v>
       </c>
       <c r="R43" s="4">
-        <v>4625</v>
+        <v>4845</v>
       </c>
       <c r="S43" s="4">
-        <v>4885</v>
+        <v>5115</v>
       </c>
       <c r="T43" s="4">
-        <v>5130</v>
+        <v>5375</v>
       </c>
       <c r="U43" s="4">
-        <v>5435</v>
+        <v>5690</v>
       </c>
       <c r="V43" s="4">
-        <v>5735</v>
+        <v>6005</v>
       </c>
       <c r="W43" s="4">
-        <v>6040</v>
+        <v>6325</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
@@ -3858,7 +3888,7 @@
         <v>1</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>6</v>
@@ -4000,70 +4030,70 @@
         <v>1</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="4">
-        <v>450</v>
+        <v>475</v>
       </c>
       <c r="E46" s="4">
-        <v>750</v>
+        <v>860</v>
       </c>
       <c r="F46" s="4">
-        <v>1060</v>
+        <v>1265</v>
       </c>
       <c r="G46" s="4">
-        <v>1390</v>
+        <v>1630</v>
       </c>
       <c r="H46" s="4">
-        <v>1705</v>
+        <v>1965</v>
       </c>
       <c r="I46" s="4">
-        <v>2025</v>
+        <v>2310</v>
       </c>
       <c r="J46" s="4">
-        <v>2345</v>
+        <v>2620</v>
       </c>
       <c r="K46" s="4">
-        <v>2660</v>
+        <v>2955</v>
       </c>
       <c r="L46" s="4">
-        <v>2960</v>
+        <v>3140</v>
       </c>
       <c r="M46" s="4">
-        <v>3235</v>
+        <v>3280</v>
       </c>
       <c r="N46" s="4">
-        <v>3490</v>
+        <v>3540</v>
       </c>
       <c r="O46" s="4">
-        <v>3770</v>
+        <v>3820</v>
       </c>
       <c r="P46" s="4">
-        <v>4040</v>
+        <v>4095</v>
       </c>
       <c r="Q46" s="4">
-        <v>4305</v>
+        <v>4365</v>
       </c>
       <c r="R46" s="4">
-        <v>4565</v>
+        <v>4625</v>
       </c>
       <c r="S46" s="4">
-        <v>4815</v>
+        <v>4885</v>
       </c>
       <c r="T46" s="4">
-        <v>5060</v>
+        <v>5130</v>
       </c>
       <c r="U46" s="4">
-        <v>5300</v>
+        <v>5435</v>
       </c>
       <c r="V46" s="4">
-        <v>5535</v>
+        <v>5735</v>
       </c>
       <c r="W46" s="4">
-        <v>5760</v>
+        <v>6040</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
@@ -4071,7 +4101,7 @@
         <v>1</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>6</v>
@@ -4142,70 +4172,70 @@
         <v>1</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="4">
-        <v>525</v>
+        <v>450</v>
       </c>
       <c r="E48" s="4">
-        <v>850</v>
+        <v>750</v>
       </c>
       <c r="F48" s="4">
-        <v>1190</v>
+        <v>1060</v>
       </c>
       <c r="G48" s="4">
-        <v>1560</v>
+        <v>1390</v>
       </c>
       <c r="H48" s="4">
-        <v>1860</v>
+        <v>1705</v>
       </c>
       <c r="I48" s="4">
-        <v>2195</v>
+        <v>2025</v>
       </c>
       <c r="J48" s="4">
-        <v>2460</v>
+        <v>2345</v>
       </c>
       <c r="K48" s="4">
-        <v>2645</v>
+        <v>2660</v>
       </c>
       <c r="L48" s="4">
-        <v>2940</v>
+        <v>2960</v>
       </c>
       <c r="M48" s="4">
-        <v>3170</v>
+        <v>3235</v>
       </c>
       <c r="N48" s="4">
-        <v>3420</v>
+        <v>3490</v>
       </c>
       <c r="O48" s="4">
-        <v>3690</v>
+        <v>3770</v>
       </c>
       <c r="P48" s="4">
-        <v>3960</v>
+        <v>4040</v>
       </c>
       <c r="Q48" s="4">
-        <v>4220</v>
+        <v>4305</v>
       </c>
       <c r="R48" s="4">
-        <v>4470</v>
+        <v>4565</v>
       </c>
       <c r="S48" s="4">
-        <v>4720</v>
+        <v>4815</v>
       </c>
       <c r="T48" s="4">
-        <v>4960</v>
+        <v>5060</v>
       </c>
       <c r="U48" s="4">
-        <v>5195</v>
+        <v>5300</v>
       </c>
       <c r="V48" s="4">
-        <v>5425</v>
+        <v>5535</v>
       </c>
       <c r="W48" s="4">
-        <v>5645</v>
+        <v>5760</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
@@ -4213,70 +4243,70 @@
         <v>1</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D49" s="4">
-        <v>575</v>
+        <v>525</v>
       </c>
       <c r="E49" s="4">
-        <v>985</v>
+        <v>850</v>
       </c>
       <c r="F49" s="4">
-        <v>1330</v>
+        <v>1190</v>
       </c>
       <c r="G49" s="4">
-        <v>1715</v>
+        <v>1560</v>
       </c>
       <c r="H49" s="4">
-        <v>2070</v>
+        <v>1860</v>
       </c>
       <c r="I49" s="4">
-        <v>2430</v>
+        <v>2195</v>
       </c>
       <c r="J49" s="4">
-        <v>2795</v>
+        <v>2460</v>
       </c>
       <c r="K49" s="4">
-        <v>3120</v>
+        <v>2645</v>
       </c>
       <c r="L49" s="4">
-        <v>3465</v>
+        <v>2940</v>
       </c>
       <c r="M49" s="4">
-        <v>3695</v>
+        <v>3170</v>
       </c>
       <c r="N49" s="4">
-        <v>3985</v>
+        <v>3420</v>
       </c>
       <c r="O49" s="4">
-        <v>4305</v>
+        <v>3690</v>
       </c>
       <c r="P49" s="4">
-        <v>4615</v>
+        <v>3960</v>
       </c>
       <c r="Q49" s="4">
-        <v>4915</v>
+        <v>4220</v>
       </c>
       <c r="R49" s="4">
-        <v>5210</v>
+        <v>4470</v>
       </c>
       <c r="S49" s="4">
-        <v>5500</v>
+        <v>4720</v>
       </c>
       <c r="T49" s="4">
-        <v>5780</v>
+        <v>4960</v>
       </c>
       <c r="U49" s="4">
-        <v>6055</v>
+        <v>5195</v>
       </c>
       <c r="V49" s="4">
-        <v>6320</v>
+        <v>5425</v>
       </c>
       <c r="W49" s="4">
-        <v>6580</v>
+        <v>5645</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
@@ -4284,70 +4314,70 @@
         <v>1</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D50" s="4">
-        <v>750</v>
+        <v>575</v>
       </c>
       <c r="E50" s="4">
-        <v>1050</v>
+        <v>985</v>
       </c>
       <c r="F50" s="4">
-        <v>1550</v>
+        <v>1330</v>
       </c>
       <c r="G50" s="4">
-        <v>2040</v>
+        <v>1715</v>
       </c>
       <c r="H50" s="4">
-        <v>2480</v>
+        <v>2070</v>
       </c>
       <c r="I50" s="4">
-        <v>2875</v>
+        <v>2430</v>
       </c>
       <c r="J50" s="4">
-        <v>3270</v>
+        <v>2795</v>
       </c>
       <c r="K50" s="4">
-        <v>3670</v>
+        <v>3120</v>
       </c>
       <c r="L50" s="4">
-        <v>3990</v>
+        <v>3465</v>
       </c>
       <c r="M50" s="4">
-        <v>4360</v>
+        <v>3695</v>
       </c>
       <c r="N50" s="4">
-        <v>4705</v>
+        <v>3985</v>
       </c>
       <c r="O50" s="4">
-        <v>5080</v>
+        <v>4305</v>
       </c>
       <c r="P50" s="4">
-        <v>5445</v>
+        <v>4615</v>
       </c>
       <c r="Q50" s="4">
-        <v>5800</v>
+        <v>4915</v>
       </c>
       <c r="R50" s="4">
-        <v>6150</v>
+        <v>5210</v>
       </c>
       <c r="S50" s="4">
-        <v>6490</v>
+        <v>5500</v>
       </c>
       <c r="T50" s="4">
-        <v>6820</v>
+        <v>5780</v>
       </c>
       <c r="U50" s="4">
-        <v>7145</v>
+        <v>6055</v>
       </c>
       <c r="V50" s="4">
-        <v>7460</v>
+        <v>6320</v>
       </c>
       <c r="W50" s="4">
-        <v>7550</v>
+        <v>6580</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
@@ -4355,70 +4385,70 @@
         <v>1</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="4">
-        <v>650</v>
+        <v>750</v>
       </c>
       <c r="E51" s="4">
-        <v>1200</v>
+        <v>1050</v>
       </c>
       <c r="F51" s="4">
-        <v>1605</v>
+        <v>1550</v>
       </c>
       <c r="G51" s="4">
-        <v>1995</v>
+        <v>2040</v>
       </c>
       <c r="H51" s="4">
-        <v>2360</v>
+        <v>2480</v>
       </c>
       <c r="I51" s="4">
-        <v>2650</v>
+        <v>2875</v>
       </c>
       <c r="J51" s="4">
-        <v>3055</v>
+        <v>3270</v>
       </c>
       <c r="K51" s="4">
-        <v>3290</v>
+        <v>3670</v>
       </c>
       <c r="L51" s="4">
-        <v>3605</v>
+        <v>3990</v>
       </c>
       <c r="M51" s="4">
-        <v>3900</v>
+        <v>4360</v>
       </c>
       <c r="N51" s="4">
-        <v>4205</v>
+        <v>4705</v>
       </c>
       <c r="O51" s="4">
-        <v>4540</v>
+        <v>5080</v>
       </c>
       <c r="P51" s="4">
-        <v>4870</v>
+        <v>5445</v>
       </c>
       <c r="Q51" s="4">
-        <v>5190</v>
+        <v>5800</v>
       </c>
       <c r="R51" s="4">
-        <v>5500</v>
+        <v>6150</v>
       </c>
       <c r="S51" s="4">
-        <v>5805</v>
+        <v>6490</v>
       </c>
       <c r="T51" s="4">
-        <v>6100</v>
+        <v>6820</v>
       </c>
       <c r="U51" s="4">
-        <v>6390</v>
+        <v>7145</v>
       </c>
       <c r="V51" s="4">
-        <v>6670</v>
+        <v>7460</v>
       </c>
       <c r="W51" s="4">
-        <v>6945</v>
+        <v>7550</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
@@ -4426,70 +4456,70 @@
         <v>1</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D52" s="4">
-        <v>575</v>
+        <v>650</v>
       </c>
       <c r="E52" s="4">
-        <v>985</v>
+        <v>1200</v>
       </c>
       <c r="F52" s="4">
-        <v>1330</v>
+        <v>1605</v>
       </c>
       <c r="G52" s="4">
-        <v>1715</v>
+        <v>1995</v>
       </c>
       <c r="H52" s="4">
-        <v>2070</v>
+        <v>2360</v>
       </c>
       <c r="I52" s="4">
-        <v>2430</v>
+        <v>2650</v>
       </c>
       <c r="J52" s="4">
-        <v>2795</v>
+        <v>3055</v>
       </c>
       <c r="K52" s="4">
-        <v>3120</v>
+        <v>3290</v>
       </c>
       <c r="L52" s="4">
-        <v>3465</v>
+        <v>3605</v>
       </c>
       <c r="M52" s="4">
-        <v>3695</v>
+        <v>3900</v>
       </c>
       <c r="N52" s="4">
-        <v>3985</v>
+        <v>4205</v>
       </c>
       <c r="O52" s="4">
-        <v>4305</v>
+        <v>4540</v>
       </c>
       <c r="P52" s="4">
-        <v>4615</v>
+        <v>4870</v>
       </c>
       <c r="Q52" s="4">
-        <v>4915</v>
+        <v>5190</v>
       </c>
       <c r="R52" s="4">
-        <v>5210</v>
+        <v>5500</v>
       </c>
       <c r="S52" s="4">
-        <v>5500</v>
+        <v>5805</v>
       </c>
       <c r="T52" s="4">
-        <v>5780</v>
+        <v>6100</v>
       </c>
       <c r="U52" s="4">
-        <v>6055</v>
+        <v>6390</v>
       </c>
       <c r="V52" s="4">
-        <v>6320</v>
+        <v>6670</v>
       </c>
       <c r="W52" s="4">
-        <v>6580</v>
+        <v>6945</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">
@@ -4497,70 +4527,70 @@
         <v>1</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D53" s="4">
-        <v>550</v>
+        <v>575</v>
       </c>
       <c r="E53" s="4">
-        <v>1020</v>
+        <v>985</v>
       </c>
       <c r="F53" s="4">
-        <v>1485</v>
+        <v>1330</v>
       </c>
       <c r="G53" s="4">
-        <v>1960</v>
+        <v>1715</v>
       </c>
       <c r="H53" s="4">
-        <v>2360</v>
+        <v>2070</v>
       </c>
       <c r="I53" s="4">
-        <v>2775</v>
+        <v>2430</v>
       </c>
       <c r="J53" s="4">
-        <v>3150</v>
+        <v>2795</v>
       </c>
       <c r="K53" s="4">
-        <v>3415</v>
+        <v>3120</v>
       </c>
       <c r="L53" s="4">
-        <v>3780</v>
+        <v>3465</v>
       </c>
       <c r="M53" s="4">
-        <v>4005</v>
+        <v>3695</v>
       </c>
       <c r="N53" s="4">
-        <v>4320</v>
+        <v>3985</v>
       </c>
       <c r="O53" s="4">
-        <v>4665</v>
+        <v>4305</v>
       </c>
       <c r="P53" s="4">
-        <v>5000</v>
+        <v>4615</v>
       </c>
       <c r="Q53" s="4">
-        <v>5330</v>
+        <v>4915</v>
       </c>
       <c r="R53" s="4">
-        <v>5650</v>
+        <v>5210</v>
       </c>
       <c r="S53" s="4">
-        <v>5960</v>
+        <v>5500</v>
       </c>
       <c r="T53" s="4">
-        <v>6265</v>
+        <v>5780</v>
       </c>
       <c r="U53" s="4">
-        <v>6565</v>
+        <v>6055</v>
       </c>
       <c r="V53" s="4">
-        <v>6850</v>
+        <v>6320</v>
       </c>
       <c r="W53" s="4">
-        <v>7130</v>
+        <v>6580</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
@@ -4568,7 +4598,7 @@
         <v>1</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>6</v>
@@ -4639,7 +4669,7 @@
         <v>1</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>6</v>
@@ -4648,61 +4678,61 @@
         <v>550</v>
       </c>
       <c r="E55" s="4">
-        <v>850</v>
+        <v>1020</v>
       </c>
       <c r="F55" s="4">
-        <v>1260</v>
+        <v>1485</v>
       </c>
       <c r="G55" s="4">
-        <v>1650</v>
+        <v>1960</v>
       </c>
       <c r="H55" s="4">
-        <v>2005</v>
+        <v>2360</v>
       </c>
       <c r="I55" s="4">
-        <v>2365</v>
+        <v>2775</v>
       </c>
       <c r="J55" s="4">
-        <v>2710</v>
+        <v>3150</v>
       </c>
       <c r="K55" s="4">
-        <v>3055</v>
+        <v>3415</v>
       </c>
       <c r="L55" s="4">
-        <v>3410</v>
+        <v>3780</v>
       </c>
       <c r="M55" s="4">
-        <v>3750</v>
+        <v>4005</v>
       </c>
       <c r="N55" s="4">
-        <v>4045</v>
+        <v>4320</v>
       </c>
       <c r="O55" s="4">
-        <v>4365</v>
+        <v>4665</v>
       </c>
       <c r="P55" s="4">
-        <v>4680</v>
+        <v>5000</v>
       </c>
       <c r="Q55" s="4">
-        <v>4990</v>
+        <v>5330</v>
       </c>
       <c r="R55" s="4">
-        <v>5290</v>
+        <v>5650</v>
       </c>
       <c r="S55" s="4">
-        <v>5580</v>
+        <v>5960</v>
       </c>
       <c r="T55" s="4">
-        <v>5865</v>
+        <v>6265</v>
       </c>
       <c r="U55" s="4">
-        <v>6145</v>
+        <v>6565</v>
       </c>
       <c r="V55" s="4">
-        <v>6415</v>
+        <v>6850</v>
       </c>
       <c r="W55" s="4">
-        <v>6675</v>
+        <v>7130</v>
       </c>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.25">
@@ -4710,7 +4740,7 @@
         <v>1</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>6</v>
@@ -4719,61 +4749,61 @@
         <v>550</v>
       </c>
       <c r="E56" s="4">
-        <v>1000</v>
+        <v>850</v>
       </c>
       <c r="F56" s="4">
-        <v>1350</v>
+        <v>1260</v>
       </c>
       <c r="G56" s="4">
-        <v>1695</v>
+        <v>1650</v>
       </c>
       <c r="H56" s="4">
-        <v>2085</v>
+        <v>2005</v>
       </c>
       <c r="I56" s="4">
-        <v>2395</v>
+        <v>2365</v>
       </c>
       <c r="J56" s="4">
-        <v>2625</v>
+        <v>2710</v>
       </c>
       <c r="K56" s="4">
-        <v>2900</v>
+        <v>3055</v>
       </c>
       <c r="L56" s="4">
-        <v>3200</v>
+        <v>3410</v>
       </c>
       <c r="M56" s="4">
-        <v>3400</v>
+        <v>3750</v>
       </c>
       <c r="N56" s="4">
-        <v>3670</v>
+        <v>4045</v>
       </c>
       <c r="O56" s="4">
-        <v>3960</v>
+        <v>4365</v>
       </c>
       <c r="P56" s="4">
-        <v>4245</v>
+        <v>4680</v>
       </c>
       <c r="Q56" s="4">
-        <v>4525</v>
+        <v>4990</v>
       </c>
       <c r="R56" s="4">
-        <v>4795</v>
+        <v>5290</v>
       </c>
       <c r="S56" s="4">
-        <v>5060</v>
+        <v>5580</v>
       </c>
       <c r="T56" s="4">
-        <v>5320</v>
+        <v>5865</v>
       </c>
       <c r="U56" s="4">
-        <v>5570</v>
+        <v>6145</v>
       </c>
       <c r="V56" s="4">
-        <v>5815</v>
+        <v>6415</v>
       </c>
       <c r="W56" s="4">
-        <v>6055</v>
+        <v>6675</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
@@ -4781,70 +4811,70 @@
         <v>1</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="4">
-        <v>575</v>
+        <v>550</v>
       </c>
       <c r="E57" s="4">
-        <v>985</v>
+        <v>1000</v>
       </c>
       <c r="F57" s="4">
-        <v>1330</v>
+        <v>1350</v>
       </c>
       <c r="G57" s="4">
-        <v>1715</v>
+        <v>1695</v>
       </c>
       <c r="H57" s="4">
-        <v>2070</v>
+        <v>2085</v>
       </c>
       <c r="I57" s="4">
-        <v>2430</v>
+        <v>2395</v>
       </c>
       <c r="J57" s="4">
-        <v>2795</v>
+        <v>2625</v>
       </c>
       <c r="K57" s="4">
-        <v>3120</v>
+        <v>2900</v>
       </c>
       <c r="L57" s="4">
-        <v>3465</v>
+        <v>3200</v>
       </c>
       <c r="M57" s="4">
-        <v>3695</v>
+        <v>3400</v>
       </c>
       <c r="N57" s="4">
-        <v>3985</v>
+        <v>3670</v>
       </c>
       <c r="O57" s="4">
-        <v>4305</v>
+        <v>3960</v>
       </c>
       <c r="P57" s="4">
-        <v>4615</v>
+        <v>4245</v>
       </c>
       <c r="Q57" s="4">
-        <v>4915</v>
+        <v>4525</v>
       </c>
       <c r="R57" s="4">
-        <v>5210</v>
+        <v>4795</v>
       </c>
       <c r="S57" s="4">
-        <v>5500</v>
+        <v>5060</v>
       </c>
       <c r="T57" s="4">
-        <v>5780</v>
+        <v>5320</v>
       </c>
       <c r="U57" s="4">
+        <v>5570</v>
+      </c>
+      <c r="V57" s="4">
+        <v>5815</v>
+      </c>
+      <c r="W57" s="4">
         <v>6055</v>
-      </c>
-      <c r="V57" s="4">
-        <v>6320</v>
-      </c>
-      <c r="W57" s="4">
-        <v>6580</v>
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
@@ -4852,7 +4882,7 @@
         <v>1</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>6</v>
@@ -4923,7 +4953,7 @@
         <v>1</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>6</v>
@@ -4994,70 +5024,70 @@
         <v>1</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D60" s="4">
-        <v>795</v>
+        <v>575</v>
       </c>
       <c r="E60" s="4">
-        <v>1280</v>
+        <v>985</v>
       </c>
       <c r="F60" s="4">
-        <v>1725</v>
+        <v>1330</v>
       </c>
       <c r="G60" s="4">
-        <v>2265</v>
+        <v>1715</v>
       </c>
       <c r="H60" s="4">
-        <v>2590</v>
+        <v>2070</v>
       </c>
       <c r="I60" s="4">
-        <v>3070</v>
+        <v>2430</v>
       </c>
       <c r="J60" s="4">
-        <v>3540</v>
+        <v>2795</v>
       </c>
       <c r="K60" s="4">
-        <v>3950</v>
+        <v>3120</v>
       </c>
       <c r="L60" s="4">
-        <v>4350</v>
+        <v>3465</v>
       </c>
       <c r="M60" s="4">
-        <v>4635</v>
+        <v>3695</v>
       </c>
       <c r="N60" s="4">
-        <v>5000</v>
+        <v>3985</v>
       </c>
       <c r="O60" s="4">
-        <v>5400</v>
+        <v>4305</v>
       </c>
       <c r="P60" s="4">
-        <v>5785</v>
+        <v>4615</v>
       </c>
       <c r="Q60" s="4">
-        <v>6165</v>
+        <v>4915</v>
       </c>
       <c r="R60" s="4">
-        <v>6540</v>
+        <v>5210</v>
       </c>
       <c r="S60" s="4">
-        <v>6900</v>
+        <v>5500</v>
       </c>
       <c r="T60" s="4">
-        <v>7250</v>
+        <v>5780</v>
       </c>
       <c r="U60" s="4">
-        <v>7595</v>
+        <v>6055</v>
       </c>
       <c r="V60" s="4">
-        <v>7850</v>
+        <v>6320</v>
       </c>
       <c r="W60" s="4">
-        <v>7920</v>
+        <v>6580</v>
       </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.25">
@@ -5065,70 +5095,70 @@
         <v>1</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="4">
-        <v>615</v>
+        <v>795</v>
       </c>
       <c r="E61" s="4">
-        <v>925</v>
+        <v>1280</v>
       </c>
       <c r="F61" s="4">
-        <v>1370</v>
+        <v>1725</v>
       </c>
       <c r="G61" s="4">
-        <v>1805</v>
+        <v>2265</v>
       </c>
       <c r="H61" s="4">
-        <v>2195</v>
+        <v>2590</v>
       </c>
       <c r="I61" s="4">
-        <v>2595</v>
+        <v>3070</v>
       </c>
       <c r="J61" s="4">
-        <v>2985</v>
+        <v>3540</v>
       </c>
       <c r="K61" s="4">
-        <v>3295</v>
+        <v>3950</v>
       </c>
       <c r="L61" s="4">
-        <v>3675</v>
+        <v>4350</v>
       </c>
       <c r="M61" s="4">
-        <v>3965</v>
+        <v>4635</v>
       </c>
       <c r="N61" s="4">
-        <v>4275</v>
+        <v>5000</v>
       </c>
       <c r="O61" s="4">
-        <v>4620</v>
+        <v>5400</v>
       </c>
       <c r="P61" s="4">
-        <v>4950</v>
+        <v>5785</v>
       </c>
       <c r="Q61" s="4">
-        <v>5275</v>
+        <v>6165</v>
       </c>
       <c r="R61" s="4">
-        <v>5595</v>
+        <v>6540</v>
       </c>
       <c r="S61" s="4">
-        <v>5900</v>
+        <v>6900</v>
       </c>
       <c r="T61" s="4">
-        <v>6205</v>
+        <v>7250</v>
       </c>
       <c r="U61" s="4">
-        <v>6495</v>
+        <v>7595</v>
       </c>
       <c r="V61" s="4">
-        <v>6785</v>
+        <v>7850</v>
       </c>
       <c r="W61" s="4">
-        <v>7060</v>
+        <v>7920</v>
       </c>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.25">
@@ -5136,7 +5166,7 @@
         <v>1</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>6</v>
@@ -5207,70 +5237,70 @@
         <v>1</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="4">
-        <v>490</v>
+        <v>615</v>
       </c>
       <c r="E63" s="4">
-        <v>695</v>
+        <v>925</v>
       </c>
       <c r="F63" s="4">
-        <v>1020</v>
+        <v>1370</v>
       </c>
       <c r="G63" s="4">
-        <v>1300</v>
+        <v>1805</v>
       </c>
       <c r="H63" s="4">
-        <v>1550</v>
+        <v>2195</v>
       </c>
       <c r="I63" s="4">
-        <v>1750</v>
+        <v>2595</v>
       </c>
       <c r="J63" s="4">
-        <v>2020</v>
+        <v>2985</v>
       </c>
       <c r="K63" s="4">
-        <v>2290</v>
+        <v>3295</v>
       </c>
       <c r="L63" s="4">
-        <v>2550</v>
+        <v>3675</v>
       </c>
       <c r="M63" s="4">
-        <v>2720</v>
+        <v>3965</v>
       </c>
       <c r="N63" s="4">
-        <v>2935</v>
+        <v>4275</v>
       </c>
       <c r="O63" s="4">
-        <v>3170</v>
+        <v>4620</v>
       </c>
       <c r="P63" s="4">
-        <v>3395</v>
+        <v>4950</v>
       </c>
       <c r="Q63" s="4">
-        <v>3620</v>
+        <v>5275</v>
       </c>
       <c r="R63" s="4">
-        <v>3840</v>
+        <v>5595</v>
       </c>
       <c r="S63" s="4">
-        <v>4050</v>
+        <v>5900</v>
       </c>
       <c r="T63" s="4">
-        <v>4255</v>
+        <v>6205</v>
       </c>
       <c r="U63" s="4">
-        <v>4460</v>
+        <v>6495</v>
       </c>
       <c r="V63" s="4">
-        <v>4655</v>
+        <v>6785</v>
       </c>
       <c r="W63" s="4">
-        <v>4845</v>
+        <v>7060</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.25">
@@ -5278,19 +5308,19 @@
         <v>1</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D64" s="4">
-        <v>540</v>
+        <v>490</v>
       </c>
       <c r="E64" s="4">
-        <v>865</v>
+        <v>695</v>
       </c>
       <c r="F64" s="4">
-        <v>1125</v>
+        <v>1020</v>
       </c>
       <c r="G64" s="4">
         <v>1300</v>
@@ -5317,31 +5347,31 @@
         <v>2935</v>
       </c>
       <c r="O64" s="4">
-        <v>2940</v>
+        <v>3170</v>
       </c>
       <c r="P64" s="4">
-        <v>3120</v>
+        <v>3395</v>
       </c>
       <c r="Q64" s="4">
-        <v>3290</v>
+        <v>3620</v>
       </c>
       <c r="R64" s="4">
-        <v>3300</v>
+        <v>3840</v>
       </c>
       <c r="S64" s="4">
-        <v>3360</v>
+        <v>4050</v>
       </c>
       <c r="T64" s="4">
-        <v>3485</v>
+        <v>4255</v>
       </c>
       <c r="U64" s="4">
-        <v>3600</v>
+        <v>4460</v>
       </c>
       <c r="V64" s="4">
-        <v>3705</v>
+        <v>4655</v>
       </c>
       <c r="W64" s="4">
-        <v>3800</v>
+        <v>4845</v>
       </c>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.25">
@@ -5349,70 +5379,70 @@
         <v>1</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="4">
-        <v>675</v>
+        <v>540</v>
       </c>
       <c r="E65" s="4">
-        <v>980</v>
+        <v>865</v>
       </c>
       <c r="F65" s="4">
-        <v>1450</v>
+        <v>1125</v>
       </c>
       <c r="G65" s="4">
-        <v>1900</v>
+        <v>1300</v>
       </c>
       <c r="H65" s="4">
-        <v>2350</v>
+        <v>1550</v>
       </c>
       <c r="I65" s="4">
-        <v>2700</v>
+        <v>1750</v>
       </c>
       <c r="J65" s="4">
-        <v>3115</v>
+        <v>2020</v>
       </c>
       <c r="K65" s="4">
-        <v>3440</v>
+        <v>2290</v>
       </c>
       <c r="L65" s="4">
-        <v>3825</v>
+        <v>2550</v>
       </c>
       <c r="M65" s="4">
-        <v>4200</v>
+        <v>2720</v>
       </c>
       <c r="N65" s="4">
-        <v>4530</v>
+        <v>2935</v>
       </c>
       <c r="O65" s="4">
-        <v>4890</v>
+        <v>2940</v>
       </c>
       <c r="P65" s="4">
-        <v>5245</v>
+        <v>3120</v>
       </c>
       <c r="Q65" s="4">
-        <v>5590</v>
+        <v>3290</v>
       </c>
       <c r="R65" s="4">
-        <v>5925</v>
+        <v>3300</v>
       </c>
       <c r="S65" s="4">
-        <v>6250</v>
+        <v>3360</v>
       </c>
       <c r="T65" s="4">
-        <v>6570</v>
+        <v>3485</v>
       </c>
       <c r="U65" s="4">
-        <v>6880</v>
+        <v>3600</v>
       </c>
       <c r="V65" s="4">
-        <v>7185</v>
+        <v>3705</v>
       </c>
       <c r="W65" s="4">
-        <v>7250</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.25">
@@ -5420,70 +5450,70 @@
         <v>1</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D66" s="4">
-        <v>750</v>
+        <v>675</v>
       </c>
       <c r="E66" s="4">
-        <v>1090</v>
+        <v>980</v>
       </c>
       <c r="F66" s="4">
-        <v>1590</v>
+        <v>1450</v>
       </c>
       <c r="G66" s="4">
-        <v>2100</v>
+        <v>1900</v>
       </c>
       <c r="H66" s="4">
-        <v>2540</v>
+        <v>2350</v>
       </c>
       <c r="I66" s="4">
-        <v>2890</v>
+        <v>2700</v>
       </c>
       <c r="J66" s="4">
-        <v>3280</v>
+        <v>3115</v>
       </c>
       <c r="K66" s="4">
-        <v>3685</v>
+        <v>3440</v>
       </c>
       <c r="L66" s="4">
-        <v>3995</v>
+        <v>3825</v>
       </c>
       <c r="M66" s="4">
-        <v>4370</v>
+        <v>4200</v>
       </c>
       <c r="N66" s="4">
-        <v>4715</v>
+        <v>4530</v>
       </c>
       <c r="O66" s="4">
-        <v>5090</v>
+        <v>4890</v>
       </c>
       <c r="P66" s="4">
-        <v>5455</v>
+        <v>5245</v>
       </c>
       <c r="Q66" s="4">
-        <v>5815</v>
+        <v>5590</v>
       </c>
       <c r="R66" s="4">
-        <v>6165</v>
+        <v>5925</v>
       </c>
       <c r="S66" s="4">
-        <v>6505</v>
+        <v>6250</v>
       </c>
       <c r="T66" s="4">
-        <v>6835</v>
+        <v>6570</v>
       </c>
       <c r="U66" s="4">
-        <v>7160</v>
+        <v>6880</v>
       </c>
       <c r="V66" s="4">
-        <v>7350</v>
+        <v>7185</v>
       </c>
       <c r="W66" s="4">
-        <v>7400</v>
+        <v>7250</v>
       </c>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.25">
@@ -5491,70 +5521,70 @@
         <v>1</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D67" s="4">
-        <v>1720</v>
+        <v>750</v>
       </c>
       <c r="E67" s="4">
-        <v>1800</v>
+        <v>1090</v>
       </c>
       <c r="F67" s="4">
-        <v>1840</v>
+        <v>1590</v>
       </c>
       <c r="G67" s="4">
-        <v>1930</v>
+        <v>2100</v>
       </c>
       <c r="H67" s="4">
-        <v>1980</v>
+        <v>2540</v>
       </c>
       <c r="I67" s="4">
-        <v>2115</v>
+        <v>2890</v>
       </c>
       <c r="J67" s="4">
-        <v>2415</v>
+        <v>3280</v>
       </c>
       <c r="K67" s="4">
-        <v>2505</v>
+        <v>3685</v>
       </c>
       <c r="L67" s="4">
-        <v>2720</v>
+        <v>3995</v>
       </c>
       <c r="M67" s="4">
-        <v>2995</v>
+        <v>4370</v>
       </c>
       <c r="N67" s="4">
-        <v>3260</v>
+        <v>4715</v>
       </c>
       <c r="O67" s="4">
-        <v>3380</v>
+        <v>5090</v>
       </c>
       <c r="P67" s="4">
-        <v>3525</v>
+        <v>5455</v>
       </c>
       <c r="Q67" s="4">
-        <v>3660</v>
+        <v>5815</v>
       </c>
       <c r="R67" s="4">
-        <v>3840</v>
+        <v>6165</v>
       </c>
       <c r="S67" s="4">
-        <v>3990</v>
+        <v>6505</v>
       </c>
       <c r="T67" s="4">
-        <v>4140</v>
+        <v>6835</v>
       </c>
       <c r="U67" s="4">
-        <v>4250</v>
+        <v>7160</v>
       </c>
       <c r="V67" s="4">
-        <v>4350</v>
+        <v>7350</v>
       </c>
       <c r="W67" s="4">
-        <v>4490</v>
+        <v>7400</v>
       </c>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.25">
@@ -5562,70 +5592,70 @@
         <v>1</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D68" s="4">
-        <v>530</v>
+        <v>1720</v>
       </c>
       <c r="E68" s="4">
-        <v>1010</v>
+        <v>1800</v>
       </c>
       <c r="F68" s="4">
-        <v>1120</v>
+        <v>1840</v>
       </c>
       <c r="G68" s="4">
-        <v>1480</v>
+        <v>1930</v>
       </c>
       <c r="H68" s="4">
-        <v>1820</v>
+        <v>1980</v>
       </c>
       <c r="I68" s="4">
-        <v>2090</v>
+        <v>2115</v>
       </c>
       <c r="J68" s="4">
-        <v>2375</v>
+        <v>2415</v>
       </c>
       <c r="K68" s="4">
-        <v>2590</v>
+        <v>2505</v>
       </c>
       <c r="L68" s="4">
         <v>2720</v>
       </c>
       <c r="M68" s="4">
-        <v>2990</v>
+        <v>2995</v>
       </c>
       <c r="N68" s="4">
-        <v>3250</v>
+        <v>3260</v>
       </c>
       <c r="O68" s="4">
-        <v>3350</v>
+        <v>3380</v>
       </c>
       <c r="P68" s="4">
-        <v>3450</v>
+        <v>3525</v>
       </c>
       <c r="Q68" s="4">
-        <v>3560</v>
+        <v>3660</v>
       </c>
       <c r="R68" s="4">
-        <v>3725</v>
+        <v>3840</v>
       </c>
       <c r="S68" s="4">
-        <v>3880</v>
+        <v>3990</v>
       </c>
       <c r="T68" s="4">
-        <v>4025</v>
+        <v>4140</v>
       </c>
       <c r="U68" s="4">
-        <v>4110</v>
+        <v>4250</v>
       </c>
       <c r="V68" s="4">
-        <v>4235</v>
+        <v>4350</v>
       </c>
       <c r="W68" s="4">
-        <v>4280</v>
+        <v>4490</v>
       </c>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.25">
@@ -5633,7 +5663,7 @@
         <v>1</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>6</v>
@@ -5642,34 +5672,34 @@
         <v>530</v>
       </c>
       <c r="E69" s="4">
-        <v>800</v>
+        <v>1010</v>
       </c>
       <c r="F69" s="4">
-        <v>1155</v>
+        <v>1120</v>
       </c>
       <c r="G69" s="4">
-        <v>1450</v>
+        <v>1480</v>
       </c>
       <c r="H69" s="4">
-        <v>1750</v>
+        <v>1820</v>
       </c>
       <c r="I69" s="4">
-        <v>2050</v>
+        <v>2090</v>
       </c>
       <c r="J69" s="4">
-        <v>2360</v>
+        <v>2375</v>
       </c>
       <c r="K69" s="4">
-        <v>2645</v>
+        <v>2590</v>
       </c>
       <c r="L69" s="4">
-        <v>2920</v>
+        <v>2720</v>
       </c>
       <c r="M69" s="4">
-        <v>3180</v>
+        <v>2990</v>
       </c>
       <c r="N69" s="4">
-        <v>3300</v>
+        <v>3250</v>
       </c>
       <c r="O69" s="4">
         <v>3350</v>
@@ -5704,7 +5734,7 @@
         <v>1</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>6</v>
@@ -5775,7 +5805,7 @@
         <v>1</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>6</v>
@@ -5845,142 +5875,142 @@
       <c r="A72" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B72" s="10" t="s">
-        <v>72</v>
+      <c r="B72" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D72" s="4">
-        <v>440</v>
+        <v>530</v>
       </c>
       <c r="E72" s="4">
-        <v>765</v>
+        <v>800</v>
       </c>
       <c r="F72" s="4">
-        <v>1040</v>
+        <v>1155</v>
       </c>
       <c r="G72" s="4">
-        <v>1360</v>
+        <v>1450</v>
       </c>
       <c r="H72" s="4">
-        <v>1635</v>
+        <v>1750</v>
       </c>
       <c r="I72" s="4">
-        <v>1830</v>
+        <v>2050</v>
       </c>
       <c r="J72" s="4">
-        <v>2080</v>
+        <v>2360</v>
       </c>
       <c r="K72" s="4">
-        <v>2335</v>
+        <v>2645</v>
       </c>
       <c r="L72" s="4">
-        <v>2530</v>
+        <v>2920</v>
       </c>
       <c r="M72" s="4">
-        <v>2750</v>
+        <v>3180</v>
       </c>
       <c r="N72" s="4">
-        <v>3000</v>
+        <v>3300</v>
       </c>
       <c r="O72" s="4">
-        <v>3100</v>
+        <v>3350</v>
       </c>
       <c r="P72" s="4">
-        <v>3250</v>
+        <v>3450</v>
       </c>
       <c r="Q72" s="4">
-        <v>3360</v>
+        <v>3560</v>
       </c>
       <c r="R72" s="4">
-        <v>3525</v>
+        <v>3725</v>
       </c>
       <c r="S72" s="4">
-        <v>3680</v>
+        <v>3880</v>
       </c>
       <c r="T72" s="4">
-        <v>3825</v>
+        <v>4025</v>
       </c>
       <c r="U72" s="4">
-        <v>3960</v>
+        <v>4110</v>
       </c>
       <c r="V72" s="4">
-        <v>4085</v>
+        <v>4235</v>
       </c>
       <c r="W72" s="4">
-        <v>4100</v>
+        <v>4280</v>
       </c>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B73" s="11" t="s">
-        <v>29</v>
+      <c r="B73" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D73" s="4">
-        <v>485</v>
+        <v>440</v>
       </c>
       <c r="E73" s="4">
-        <v>695</v>
+        <v>765</v>
       </c>
       <c r="F73" s="4">
-        <v>975</v>
+        <v>1040</v>
       </c>
       <c r="G73" s="4">
-        <v>1150</v>
+        <v>1360</v>
       </c>
       <c r="H73" s="4">
-        <v>1325</v>
+        <v>1635</v>
       </c>
       <c r="I73" s="4">
-        <v>1485</v>
+        <v>1830</v>
       </c>
       <c r="J73" s="4">
-        <v>1690</v>
+        <v>2080</v>
       </c>
       <c r="K73" s="4">
-        <v>1800</v>
+        <v>2335</v>
       </c>
       <c r="L73" s="4">
-        <v>1990</v>
+        <v>2530</v>
       </c>
       <c r="M73" s="4">
-        <v>2085</v>
+        <v>2750</v>
       </c>
       <c r="N73" s="4">
-        <v>2250</v>
+        <v>3000</v>
       </c>
       <c r="O73" s="4">
-        <v>2430</v>
+        <v>3100</v>
       </c>
       <c r="P73" s="4">
-        <v>2605</v>
+        <v>3250</v>
       </c>
       <c r="Q73" s="4">
-        <v>2775</v>
+        <v>3360</v>
       </c>
       <c r="R73" s="4">
-        <v>2940</v>
+        <v>3525</v>
       </c>
       <c r="S73" s="4">
-        <v>3105</v>
+        <v>3680</v>
       </c>
       <c r="T73" s="4">
-        <v>3265</v>
+        <v>3825</v>
       </c>
       <c r="U73" s="4">
-        <v>3420</v>
+        <v>3960</v>
       </c>
       <c r="V73" s="4">
-        <v>3570</v>
+        <v>4085</v>
       </c>
       <c r="W73" s="4">
-        <v>3715</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.25">
@@ -5988,70 +6018,70 @@
         <v>1</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D74" s="4">
-        <v>540</v>
+        <v>485</v>
       </c>
       <c r="E74" s="4">
-        <v>800</v>
+        <v>695</v>
       </c>
       <c r="F74" s="4">
-        <v>1035</v>
+        <v>975</v>
       </c>
       <c r="G74" s="4">
-        <v>1375</v>
+        <v>1150</v>
       </c>
       <c r="H74" s="4">
-        <v>1585</v>
+        <v>1325</v>
       </c>
       <c r="I74" s="4">
-        <v>1870</v>
+        <v>1485</v>
       </c>
       <c r="J74" s="4">
-        <v>2160</v>
+        <v>1690</v>
       </c>
       <c r="K74" s="4">
-        <v>2440</v>
+        <v>1800</v>
       </c>
       <c r="L74" s="4">
-        <v>2730</v>
+        <v>1990</v>
       </c>
       <c r="M74" s="4">
-        <v>2985</v>
+        <v>2085</v>
       </c>
       <c r="N74" s="4">
-        <v>3220</v>
+        <v>2250</v>
       </c>
       <c r="O74" s="4">
-        <v>3475</v>
+        <v>2430</v>
       </c>
       <c r="P74" s="4">
-        <v>3550</v>
+        <v>2605</v>
       </c>
       <c r="Q74" s="4">
-        <v>3620</v>
+        <v>2775</v>
       </c>
       <c r="R74" s="4">
-        <v>3680</v>
+        <v>2940</v>
       </c>
       <c r="S74" s="4">
-        <v>3750</v>
+        <v>3105</v>
       </c>
       <c r="T74" s="4">
-        <v>3820</v>
+        <v>3265</v>
       </c>
       <c r="U74" s="4">
-        <v>3900</v>
+        <v>3420</v>
       </c>
       <c r="V74" s="4">
-        <v>3940</v>
+        <v>3570</v>
       </c>
       <c r="W74" s="4">
-        <v>3980</v>
+        <v>3715</v>
       </c>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.25">
@@ -6059,7 +6089,7 @@
         <v>1</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>6</v>
@@ -6130,16 +6160,16 @@
         <v>1</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D76" s="4">
-        <v>485</v>
+        <v>540</v>
       </c>
       <c r="E76" s="4">
-        <v>695</v>
+        <v>800</v>
       </c>
       <c r="F76" s="4">
         <v>1035</v>
@@ -6166,7 +6196,7 @@
         <v>2985</v>
       </c>
       <c r="N76" s="4">
-        <v>2990</v>
+        <v>3220</v>
       </c>
       <c r="O76" s="4">
         <v>3475</v>
@@ -6201,70 +6231,70 @@
         <v>1</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D77" s="4">
-        <v>615</v>
+        <v>485</v>
       </c>
       <c r="E77" s="4">
-        <v>840</v>
+        <v>695</v>
       </c>
       <c r="F77" s="4">
-        <v>1150</v>
+        <v>1035</v>
       </c>
       <c r="G77" s="4">
-        <v>1500</v>
+        <v>1375</v>
       </c>
       <c r="H77" s="4">
-        <v>1705</v>
+        <v>1585</v>
       </c>
       <c r="I77" s="4">
-        <v>2025</v>
+        <v>1870</v>
       </c>
       <c r="J77" s="4">
-        <v>2345</v>
+        <v>2160</v>
       </c>
       <c r="K77" s="4">
-        <v>2660</v>
+        <v>2440</v>
       </c>
       <c r="L77" s="4">
-        <v>2960</v>
+        <v>2730</v>
       </c>
       <c r="M77" s="4">
-        <v>3235</v>
+        <v>2985</v>
       </c>
       <c r="N77" s="4">
-        <v>3490</v>
+        <v>2990</v>
       </c>
       <c r="O77" s="4">
-        <v>3770</v>
+        <v>3475</v>
       </c>
       <c r="P77" s="4">
-        <v>4040</v>
+        <v>3550</v>
       </c>
       <c r="Q77" s="4">
-        <v>4305</v>
+        <v>3620</v>
       </c>
       <c r="R77" s="4">
-        <v>4565</v>
+        <v>3680</v>
       </c>
       <c r="S77" s="4">
-        <v>4815</v>
+        <v>3750</v>
       </c>
       <c r="T77" s="4">
-        <v>5060</v>
+        <v>3820</v>
       </c>
       <c r="U77" s="4">
-        <v>5300</v>
+        <v>3900</v>
       </c>
       <c r="V77" s="4">
-        <v>5535</v>
+        <v>3940</v>
       </c>
       <c r="W77" s="4">
-        <v>5760</v>
+        <v>3980</v>
       </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.25">
@@ -6272,70 +6302,70 @@
         <v>1</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D78" s="4">
-        <v>240</v>
+        <v>615</v>
       </c>
       <c r="E78" s="4">
-        <v>430</v>
+        <v>840</v>
       </c>
       <c r="F78" s="4">
-        <v>550</v>
+        <v>1150</v>
       </c>
       <c r="G78" s="4">
-        <v>570</v>
+        <v>1500</v>
       </c>
       <c r="H78" s="4">
-        <v>590</v>
+        <v>1705</v>
       </c>
       <c r="I78" s="4">
-        <v>590</v>
+        <v>2025</v>
       </c>
       <c r="J78" s="4">
-        <v>590</v>
+        <v>2345</v>
       </c>
       <c r="K78" s="4">
-        <v>650</v>
+        <v>2660</v>
       </c>
       <c r="L78" s="4">
-        <v>705</v>
+        <v>2960</v>
       </c>
       <c r="M78" s="4">
-        <v>765</v>
+        <v>3235</v>
       </c>
       <c r="N78" s="4">
-        <v>820</v>
+        <v>3490</v>
       </c>
       <c r="O78" s="4">
-        <v>875</v>
+        <v>3770</v>
       </c>
       <c r="P78" s="4">
-        <v>900</v>
+        <v>4040</v>
       </c>
       <c r="Q78" s="4">
-        <v>930</v>
+        <v>4305</v>
       </c>
       <c r="R78" s="4">
-        <v>955</v>
+        <v>4565</v>
       </c>
       <c r="S78" s="4">
-        <v>985</v>
+        <v>4815</v>
       </c>
       <c r="T78" s="4">
-        <v>1010</v>
+        <v>5060</v>
       </c>
       <c r="U78" s="4">
-        <v>1035</v>
+        <v>5300</v>
       </c>
       <c r="V78" s="4">
-        <v>1095</v>
+        <v>5535</v>
       </c>
       <c r="W78" s="4">
-        <v>1150</v>
+        <v>5760</v>
       </c>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
@@ -6343,7 +6373,7 @@
         <v>1</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>4</v>
@@ -6352,10 +6382,10 @@
         <v>240</v>
       </c>
       <c r="E79" s="4">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="F79" s="4">
-        <v>525</v>
+        <v>550</v>
       </c>
       <c r="G79" s="4">
         <v>570</v>
@@ -6414,70 +6444,70 @@
         <v>1</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D80" s="4">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="E80" s="4">
-        <v>370</v>
+        <v>445</v>
       </c>
       <c r="F80" s="4">
-        <v>385</v>
+        <v>525</v>
       </c>
       <c r="G80" s="4">
-        <v>540</v>
+        <v>570</v>
       </c>
       <c r="H80" s="4">
-        <v>535</v>
+        <v>590</v>
       </c>
       <c r="I80" s="4">
-        <v>535</v>
+        <v>590</v>
       </c>
       <c r="J80" s="4">
-        <v>550</v>
+        <v>590</v>
       </c>
       <c r="K80" s="4">
-        <v>555</v>
+        <v>650</v>
       </c>
       <c r="L80" s="4">
-        <v>565</v>
+        <v>705</v>
       </c>
       <c r="M80" s="4">
-        <v>575</v>
+        <v>765</v>
       </c>
       <c r="N80" s="4">
-        <v>585</v>
+        <v>820</v>
       </c>
       <c r="O80" s="4">
-        <v>585</v>
+        <v>875</v>
       </c>
       <c r="P80" s="4">
-        <v>580</v>
+        <v>900</v>
       </c>
       <c r="Q80" s="4">
-        <v>580</v>
+        <v>930</v>
       </c>
       <c r="R80" s="4">
-        <v>580</v>
+        <v>955</v>
       </c>
       <c r="S80" s="4">
-        <v>580</v>
+        <v>985</v>
       </c>
       <c r="T80" s="4">
-        <v>580</v>
+        <v>1010</v>
       </c>
       <c r="U80" s="4">
-        <v>580</v>
+        <v>1035</v>
       </c>
       <c r="V80" s="4">
-        <v>580</v>
+        <v>1095</v>
       </c>
       <c r="W80" s="4">
-        <v>580</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.25">
@@ -6485,70 +6515,70 @@
         <v>1</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D81" s="4">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E81" s="4">
-        <v>450</v>
+        <v>370</v>
       </c>
       <c r="F81" s="4">
+        <v>385</v>
+      </c>
+      <c r="G81" s="4">
         <v>540</v>
       </c>
-      <c r="G81" s="4">
-        <v>570</v>
-      </c>
       <c r="H81" s="4">
-        <v>590</v>
+        <v>535</v>
       </c>
       <c r="I81" s="4">
-        <v>590</v>
+        <v>535</v>
       </c>
       <c r="J81" s="4">
-        <v>590</v>
+        <v>550</v>
       </c>
       <c r="K81" s="4">
-        <v>650</v>
+        <v>555</v>
       </c>
       <c r="L81" s="4">
-        <v>705</v>
+        <v>565</v>
       </c>
       <c r="M81" s="4">
-        <v>765</v>
+        <v>575</v>
       </c>
       <c r="N81" s="4">
-        <v>820</v>
+        <v>585</v>
       </c>
       <c r="O81" s="4">
-        <v>875</v>
+        <v>585</v>
       </c>
       <c r="P81" s="4">
-        <v>900</v>
+        <v>580</v>
       </c>
       <c r="Q81" s="4">
-        <v>930</v>
+        <v>580</v>
       </c>
       <c r="R81" s="4">
-        <v>955</v>
+        <v>580</v>
       </c>
       <c r="S81" s="4">
-        <v>985</v>
+        <v>580</v>
       </c>
       <c r="T81" s="4">
-        <v>1010</v>
+        <v>580</v>
       </c>
       <c r="U81" s="4">
-        <v>1035</v>
+        <v>580</v>
       </c>
       <c r="V81" s="4">
-        <v>1095</v>
+        <v>580</v>
       </c>
       <c r="W81" s="4">
-        <v>1150</v>
+        <v>580</v>
       </c>
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.25">
@@ -6556,70 +6586,70 @@
         <v>1</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D82" s="4">
-        <v>60</v>
+        <v>240</v>
       </c>
       <c r="E82" s="4">
-        <v>105</v>
+        <v>450</v>
       </c>
       <c r="F82" s="4">
-        <v>145</v>
+        <v>540</v>
       </c>
       <c r="G82" s="4">
-        <v>180</v>
+        <v>570</v>
       </c>
       <c r="H82" s="4">
-        <v>240</v>
+        <v>590</v>
       </c>
       <c r="I82" s="4">
-        <v>295</v>
+        <v>590</v>
       </c>
       <c r="J82" s="4">
-        <v>295</v>
+        <v>590</v>
       </c>
       <c r="K82" s="4">
-        <v>295</v>
+        <v>650</v>
       </c>
       <c r="L82" s="4">
-        <v>295</v>
+        <v>705</v>
       </c>
       <c r="M82" s="4">
-        <v>295</v>
+        <v>765</v>
       </c>
       <c r="N82" s="4">
-        <v>295</v>
+        <v>820</v>
       </c>
       <c r="O82" s="4">
-        <v>295</v>
+        <v>875</v>
       </c>
       <c r="P82" s="4">
-        <v>295</v>
+        <v>900</v>
       </c>
       <c r="Q82" s="4">
-        <v>295</v>
+        <v>930</v>
       </c>
       <c r="R82" s="4">
-        <v>295</v>
+        <v>955</v>
       </c>
       <c r="S82" s="4">
-        <v>325</v>
+        <v>985</v>
       </c>
       <c r="T82" s="4">
-        <v>325</v>
+        <v>1010</v>
       </c>
       <c r="U82" s="4">
-        <v>325</v>
+        <v>1035</v>
       </c>
       <c r="V82" s="4">
-        <v>325</v>
+        <v>1095</v>
       </c>
       <c r="W82" s="4">
-        <v>325</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.25">
@@ -6627,7 +6657,7 @@
         <v>1</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>4</v>
@@ -6698,70 +6728,70 @@
         <v>1</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D84" s="4">
-        <v>355</v>
+        <v>60</v>
       </c>
       <c r="E84" s="4">
-        <v>635</v>
+        <v>105</v>
       </c>
       <c r="F84" s="4">
-        <v>835</v>
+        <v>145</v>
       </c>
       <c r="G84" s="4">
-        <v>925</v>
+        <v>180</v>
       </c>
       <c r="H84" s="4">
-        <v>1035</v>
+        <v>240</v>
       </c>
       <c r="I84" s="4">
-        <v>1240</v>
+        <v>295</v>
       </c>
       <c r="J84" s="4">
-        <v>1400</v>
+        <v>295</v>
       </c>
       <c r="K84" s="4">
-        <v>1600</v>
+        <v>295</v>
       </c>
       <c r="L84" s="4">
-        <v>1740</v>
+        <v>295</v>
       </c>
       <c r="M84" s="4">
-        <v>1935</v>
+        <v>295</v>
       </c>
       <c r="N84" s="4">
-        <v>2040</v>
+        <v>295</v>
       </c>
       <c r="O84" s="4">
-        <v>2160</v>
+        <v>295</v>
       </c>
       <c r="P84" s="4">
-        <v>2265</v>
+        <v>295</v>
       </c>
       <c r="Q84" s="4">
-        <v>2380</v>
+        <v>295</v>
       </c>
       <c r="R84" s="4">
-        <v>2485</v>
+        <v>295</v>
       </c>
       <c r="S84" s="4">
-        <v>2600</v>
+        <v>325</v>
       </c>
       <c r="T84" s="4">
-        <v>0</v>
+        <v>325</v>
       </c>
       <c r="U84" s="4">
-        <v>0</v>
+        <v>325</v>
       </c>
       <c r="V84" s="4">
-        <v>0</v>
+        <v>325</v>
       </c>
       <c r="W84" s="4">
-        <v>0</v>
+        <v>325</v>
       </c>
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.25">
@@ -6769,70 +6799,70 @@
         <v>1</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D85" s="4">
-        <v>420</v>
+        <v>355</v>
       </c>
       <c r="E85" s="4">
-        <v>660</v>
+        <v>635</v>
       </c>
       <c r="F85" s="4">
-        <v>985</v>
+        <v>835</v>
       </c>
       <c r="G85" s="4">
-        <v>1190</v>
+        <v>925</v>
       </c>
       <c r="H85" s="4">
-        <v>1475</v>
+        <v>1035</v>
       </c>
       <c r="I85" s="4">
-        <v>1770</v>
+        <v>1240</v>
       </c>
       <c r="J85" s="4">
-        <v>2060</v>
+        <v>1400</v>
       </c>
       <c r="K85" s="4">
-        <v>2350</v>
+        <v>1600</v>
       </c>
       <c r="L85" s="4">
-        <v>2635</v>
+        <v>1740</v>
       </c>
       <c r="M85" s="4">
-        <v>2925</v>
+        <v>1935</v>
       </c>
       <c r="N85" s="4">
-        <v>3205</v>
+        <v>2040</v>
       </c>
       <c r="O85" s="4">
-        <v>3495</v>
+        <v>2160</v>
       </c>
       <c r="P85" s="4">
-        <v>3770</v>
+        <v>2265</v>
       </c>
       <c r="Q85" s="4">
-        <v>4060</v>
+        <v>2380</v>
       </c>
       <c r="R85" s="4">
-        <v>4335</v>
+        <v>2485</v>
       </c>
       <c r="S85" s="4">
-        <v>4620</v>
+        <v>2600</v>
       </c>
       <c r="T85" s="4">
-        <v>4890</v>
+        <v>0</v>
       </c>
       <c r="U85" s="4">
-        <v>5175</v>
+        <v>0</v>
       </c>
       <c r="V85" s="4">
-        <v>5465</v>
+        <v>0</v>
       </c>
       <c r="W85" s="4">
-        <v>5750</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.25">
@@ -6840,7 +6870,7 @@
         <v>1</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>4</v>
@@ -6911,70 +6941,70 @@
         <v>1</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D87" s="4">
-        <v>440</v>
+        <v>420</v>
       </c>
       <c r="E87" s="4">
-        <v>725</v>
+        <v>660</v>
       </c>
       <c r="F87" s="4">
-        <v>800</v>
+        <v>985</v>
       </c>
       <c r="G87" s="4">
-        <v>840</v>
+        <v>1190</v>
       </c>
       <c r="H87" s="4">
-        <v>860</v>
+        <v>1475</v>
       </c>
       <c r="I87" s="4">
-        <v>1030</v>
+        <v>1770</v>
       </c>
       <c r="J87" s="4">
-        <v>1195</v>
+        <v>2060</v>
       </c>
       <c r="K87" s="4">
-        <v>1365</v>
+        <v>2350</v>
       </c>
       <c r="L87" s="4">
-        <v>1530</v>
+        <v>2635</v>
       </c>
       <c r="M87" s="4">
-        <v>1700</v>
+        <v>2925</v>
       </c>
       <c r="N87" s="4">
-        <v>1860</v>
+        <v>3205</v>
       </c>
       <c r="O87" s="4">
-        <v>2030</v>
+        <v>3495</v>
       </c>
       <c r="P87" s="4">
-        <v>2190</v>
+        <v>3770</v>
       </c>
       <c r="Q87" s="4">
-        <v>2355</v>
+        <v>4060</v>
       </c>
       <c r="R87" s="4">
-        <v>2515</v>
+        <v>4335</v>
       </c>
       <c r="S87" s="4">
-        <v>2680</v>
+        <v>4620</v>
       </c>
       <c r="T87" s="4">
-        <v>2835</v>
+        <v>4890</v>
       </c>
       <c r="U87" s="4">
-        <v>3005</v>
+        <v>5175</v>
       </c>
       <c r="V87" s="4">
-        <v>3170</v>
+        <v>5465</v>
       </c>
       <c r="W87" s="4">
-        <v>3335</v>
+        <v>5750</v>
       </c>
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.25">
@@ -6982,16 +7012,16 @@
         <v>1</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D88" s="4">
-        <v>460</v>
+        <v>440</v>
       </c>
       <c r="E88" s="4">
-        <v>750</v>
+        <v>725</v>
       </c>
       <c r="F88" s="4">
         <v>800</v>
@@ -7053,70 +7083,70 @@
         <v>1</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D89" s="4">
-        <v>425</v>
+        <v>460</v>
       </c>
       <c r="E89" s="4">
-        <v>695</v>
+        <v>750</v>
       </c>
       <c r="F89" s="4">
-        <v>750</v>
+        <v>800</v>
       </c>
       <c r="G89" s="4">
-        <v>895</v>
+        <v>840</v>
       </c>
       <c r="H89" s="4">
-        <v>1035</v>
+        <v>860</v>
       </c>
       <c r="I89" s="4">
-        <v>1180</v>
+        <v>1030</v>
       </c>
       <c r="J89" s="4">
-        <v>1295</v>
+        <v>1195</v>
       </c>
       <c r="K89" s="4">
-        <v>1485</v>
+        <v>1365</v>
       </c>
       <c r="L89" s="4">
-        <v>1580</v>
+        <v>1530</v>
       </c>
       <c r="M89" s="4">
-        <v>1640</v>
+        <v>1700</v>
       </c>
       <c r="N89" s="4">
-        <v>1690</v>
+        <v>1860</v>
       </c>
       <c r="O89" s="4">
-        <v>1750</v>
+        <v>2030</v>
       </c>
       <c r="P89" s="4">
-        <v>1800</v>
+        <v>2190</v>
       </c>
       <c r="Q89" s="4">
-        <v>1860</v>
+        <v>2355</v>
       </c>
       <c r="R89" s="4">
-        <v>1910</v>
+        <v>2515</v>
       </c>
       <c r="S89" s="4">
-        <v>1965</v>
+        <v>2680</v>
       </c>
       <c r="T89" s="4">
-        <v>2015</v>
+        <v>2835</v>
       </c>
       <c r="U89" s="4">
-        <v>2070</v>
+        <v>3005</v>
       </c>
       <c r="V89" s="4">
-        <v>2130</v>
+        <v>3170</v>
       </c>
       <c r="W89" s="4">
-        <v>2185</v>
+        <v>3335</v>
       </c>
     </row>
     <row r="90" spans="1:23" x14ac:dyDescent="0.25">
@@ -7124,70 +7154,70 @@
         <v>1</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D90" s="4">
-        <v>450</v>
+        <v>425</v>
       </c>
       <c r="E90" s="4">
-        <v>725</v>
+        <v>695</v>
       </c>
       <c r="F90" s="4">
-        <v>775</v>
+        <v>750</v>
       </c>
       <c r="G90" s="4">
-        <v>825</v>
+        <v>895</v>
       </c>
       <c r="H90" s="4">
-        <v>860</v>
+        <v>1035</v>
       </c>
       <c r="I90" s="4">
-        <v>1030</v>
+        <v>1180</v>
       </c>
       <c r="J90" s="4">
-        <v>1195</v>
+        <v>1295</v>
       </c>
       <c r="K90" s="4">
-        <v>1365</v>
+        <v>1485</v>
       </c>
       <c r="L90" s="4">
-        <v>1530</v>
+        <v>1580</v>
       </c>
       <c r="M90" s="4">
-        <v>1700</v>
+        <v>1640</v>
       </c>
       <c r="N90" s="4">
+        <v>1690</v>
+      </c>
+      <c r="O90" s="4">
+        <v>1750</v>
+      </c>
+      <c r="P90" s="4">
+        <v>1800</v>
+      </c>
+      <c r="Q90" s="4">
         <v>1860</v>
       </c>
-      <c r="O90" s="4">
-        <v>2030</v>
-      </c>
-      <c r="P90" s="4">
-        <v>2190</v>
-      </c>
-      <c r="Q90" s="4">
-        <v>2355</v>
-      </c>
       <c r="R90" s="4">
-        <v>2515</v>
+        <v>1910</v>
       </c>
       <c r="S90" s="4">
-        <v>2680</v>
+        <v>1965</v>
       </c>
       <c r="T90" s="4">
-        <v>2835</v>
+        <v>2015</v>
       </c>
       <c r="U90" s="4">
-        <v>3005</v>
+        <v>2070</v>
       </c>
       <c r="V90" s="4">
-        <v>3170</v>
+        <v>2130</v>
       </c>
       <c r="W90" s="4">
-        <v>3335</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.25">
@@ -7195,70 +7225,70 @@
         <v>1</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D91" s="4">
-        <v>195</v>
+        <v>450</v>
       </c>
       <c r="E91" s="4">
-        <v>320</v>
+        <v>725</v>
       </c>
       <c r="F91" s="4">
-        <v>480</v>
+        <v>775</v>
       </c>
       <c r="G91" s="4">
-        <v>595</v>
+        <v>825</v>
       </c>
       <c r="H91" s="4">
-        <v>620</v>
+        <v>860</v>
       </c>
       <c r="I91" s="4">
-        <v>650</v>
+        <v>1030</v>
       </c>
       <c r="J91" s="4">
-        <v>680</v>
+        <v>1195</v>
       </c>
       <c r="K91" s="4">
-        <v>705</v>
+        <v>1365</v>
       </c>
       <c r="L91" s="4">
-        <v>735</v>
+        <v>1530</v>
       </c>
       <c r="M91" s="4">
-        <v>765</v>
+        <v>1700</v>
       </c>
       <c r="N91" s="4">
-        <v>790</v>
+        <v>1860</v>
       </c>
       <c r="O91" s="4">
-        <v>820</v>
+        <v>2030</v>
       </c>
       <c r="P91" s="4">
-        <v>845</v>
+        <v>2190</v>
       </c>
       <c r="Q91" s="4">
-        <v>870</v>
+        <v>2355</v>
       </c>
       <c r="R91" s="4">
-        <v>900</v>
+        <v>2515</v>
       </c>
       <c r="S91" s="4">
-        <v>925</v>
+        <v>2680</v>
       </c>
       <c r="T91" s="4">
-        <v>950</v>
+        <v>2835</v>
       </c>
       <c r="U91" s="4">
-        <v>980</v>
+        <v>3005</v>
       </c>
       <c r="V91" s="4">
-        <v>1010</v>
+        <v>3170</v>
       </c>
       <c r="W91" s="4">
-        <v>1035</v>
+        <v>3335</v>
       </c>
     </row>
     <row r="92" spans="1:23" x14ac:dyDescent="0.25">
@@ -7266,70 +7296,70 @@
         <v>1</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D92" s="4">
-        <v>315</v>
+        <v>195</v>
       </c>
       <c r="E92" s="4">
-        <v>560</v>
+        <v>320</v>
       </c>
       <c r="F92" s="4">
-        <v>840</v>
+        <v>480</v>
       </c>
       <c r="G92" s="4">
-        <v>1190</v>
+        <v>595</v>
       </c>
       <c r="H92" s="4">
-        <v>1180</v>
+        <v>620</v>
       </c>
       <c r="I92" s="4">
-        <v>1225</v>
+        <v>650</v>
       </c>
       <c r="J92" s="4">
-        <v>1465</v>
+        <v>680</v>
       </c>
       <c r="K92" s="4">
-        <v>1470</v>
+        <v>705</v>
       </c>
       <c r="L92" s="4">
-        <v>1570</v>
+        <v>735</v>
       </c>
       <c r="M92" s="4">
-        <v>1775</v>
+        <v>765</v>
       </c>
       <c r="N92" s="4">
-        <v>1785</v>
+        <v>790</v>
       </c>
       <c r="O92" s="4">
-        <v>1865</v>
+        <v>820</v>
       </c>
       <c r="P92" s="4">
-        <v>2055</v>
+        <v>845</v>
       </c>
       <c r="Q92" s="4">
-        <v>2240</v>
+        <v>870</v>
       </c>
       <c r="R92" s="4">
-        <v>2080</v>
+        <v>900</v>
       </c>
       <c r="S92" s="4">
-        <v>2255</v>
+        <v>925</v>
       </c>
       <c r="T92" s="4">
-        <v>2410</v>
+        <v>950</v>
       </c>
       <c r="U92" s="4">
-        <v>2500</v>
+        <v>980</v>
       </c>
       <c r="V92" s="4">
-        <v>2590</v>
+        <v>1010</v>
       </c>
       <c r="W92" s="4">
-        <v>2695</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="93" spans="1:23" x14ac:dyDescent="0.25">
@@ -7337,19 +7367,19 @@
         <v>1</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D93" s="4">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="E93" s="4">
-        <v>625</v>
+        <v>560</v>
       </c>
       <c r="F93" s="4">
-        <v>940</v>
+        <v>840</v>
       </c>
       <c r="G93" s="4">
         <v>1190</v>
@@ -7397,10 +7427,10 @@
         <v>2500</v>
       </c>
       <c r="V93" s="4">
-        <v>0</v>
+        <v>2590</v>
       </c>
       <c r="W93" s="4">
-        <v>0</v>
+        <v>2695</v>
       </c>
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.25">
@@ -7408,70 +7438,70 @@
         <v>1</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D94" s="4">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="E94" s="4">
-        <v>600</v>
+        <v>625</v>
       </c>
       <c r="F94" s="4">
-        <v>650</v>
+        <v>940</v>
       </c>
       <c r="G94" s="4">
-        <v>715</v>
+        <v>1190</v>
       </c>
       <c r="H94" s="4">
-        <v>830</v>
+        <v>1180</v>
       </c>
       <c r="I94" s="4">
-        <v>945</v>
+        <v>1225</v>
       </c>
       <c r="J94" s="4">
-        <v>1060</v>
+        <v>1465</v>
       </c>
       <c r="K94" s="4">
-        <v>1175</v>
+        <v>1470</v>
       </c>
       <c r="L94" s="4">
-        <v>1260</v>
+        <v>1570</v>
       </c>
       <c r="M94" s="4">
-        <v>1350</v>
+        <v>1775</v>
       </c>
       <c r="N94" s="4">
-        <v>1460</v>
+        <v>1785</v>
       </c>
       <c r="O94" s="4">
-        <v>1575</v>
+        <v>1865</v>
       </c>
       <c r="P94" s="4">
-        <v>1685</v>
+        <v>2055</v>
       </c>
       <c r="Q94" s="4">
-        <v>1770</v>
+        <v>2240</v>
       </c>
       <c r="R94" s="4">
-        <v>1850</v>
+        <v>2080</v>
       </c>
       <c r="S94" s="4">
-        <v>1910</v>
+        <v>2255</v>
       </c>
       <c r="T94" s="4">
-        <v>1955</v>
+        <v>2410</v>
       </c>
       <c r="U94" s="4">
-        <v>2070</v>
+        <v>2500</v>
       </c>
       <c r="V94" s="4">
-        <v>2185</v>
+        <v>0</v>
       </c>
       <c r="W94" s="4">
-        <v>2300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:23" x14ac:dyDescent="0.25">
@@ -7479,70 +7509,70 @@
         <v>1</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D95" s="4">
-        <v>275</v>
+        <v>350</v>
       </c>
       <c r="E95" s="4">
-        <v>485</v>
+        <v>600</v>
       </c>
       <c r="F95" s="4">
-        <v>720</v>
+        <v>650</v>
       </c>
       <c r="G95" s="4">
-        <v>1075</v>
+        <v>715</v>
       </c>
       <c r="H95" s="4">
-        <v>1065</v>
+        <v>830</v>
       </c>
       <c r="I95" s="4">
-        <v>1065</v>
+        <v>945</v>
       </c>
       <c r="J95" s="4">
-        <v>1090</v>
+        <v>1060</v>
       </c>
       <c r="K95" s="4">
-        <v>1105</v>
+        <v>1175</v>
       </c>
       <c r="L95" s="4">
-        <v>1170</v>
+        <v>1260</v>
       </c>
       <c r="M95" s="4">
-        <v>1335</v>
+        <v>1350</v>
       </c>
       <c r="N95" s="4">
-        <v>1340</v>
+        <v>1460</v>
       </c>
       <c r="O95" s="4">
-        <v>1400</v>
+        <v>1575</v>
       </c>
       <c r="P95" s="4">
-        <v>1545</v>
+        <v>1685</v>
       </c>
       <c r="Q95" s="4">
-        <v>1685</v>
+        <v>1770</v>
       </c>
       <c r="R95" s="4">
-        <v>1575</v>
+        <v>1850</v>
       </c>
       <c r="S95" s="4">
-        <v>1700</v>
+        <v>1910</v>
       </c>
       <c r="T95" s="4">
-        <v>1820</v>
+        <v>1955</v>
       </c>
       <c r="U95" s="4">
-        <v>1885</v>
+        <v>2070</v>
       </c>
       <c r="V95" s="4">
-        <v>0</v>
+        <v>2185</v>
       </c>
       <c r="W95" s="4">
-        <v>0</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="96" spans="1:23" x14ac:dyDescent="0.25">
@@ -7550,70 +7580,70 @@
         <v>1</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D96" s="4">
-        <v>440</v>
+        <v>275</v>
       </c>
       <c r="E96" s="4">
-        <v>600</v>
+        <v>485</v>
       </c>
       <c r="F96" s="4">
-        <v>595</v>
+        <v>720</v>
       </c>
       <c r="G96" s="4">
-        <v>715</v>
+        <v>1075</v>
       </c>
       <c r="H96" s="4">
-        <v>885</v>
+        <v>1065</v>
       </c>
       <c r="I96" s="4">
         <v>1065</v>
       </c>
       <c r="J96" s="4">
-        <v>1205</v>
+        <v>1090</v>
       </c>
       <c r="K96" s="4">
-        <v>1355</v>
+        <v>1105</v>
       </c>
       <c r="L96" s="4">
-        <v>1495</v>
+        <v>1170</v>
       </c>
       <c r="M96" s="4">
-        <v>1640</v>
+        <v>1335</v>
       </c>
       <c r="N96" s="4">
-        <v>1750</v>
+        <v>1340</v>
       </c>
       <c r="O96" s="4">
-        <v>1865</v>
+        <v>1400</v>
       </c>
       <c r="P96" s="4">
-        <v>1975</v>
+        <v>1545</v>
       </c>
       <c r="Q96" s="4">
-        <v>2090</v>
+        <v>1685</v>
       </c>
       <c r="R96" s="4">
-        <v>2195</v>
+        <v>1575</v>
       </c>
       <c r="S96" s="4">
-        <v>2310</v>
+        <v>1700</v>
       </c>
       <c r="T96" s="4">
-        <v>2415</v>
+        <v>1820</v>
       </c>
       <c r="U96" s="4">
-        <v>2530</v>
+        <v>1885</v>
       </c>
       <c r="V96" s="4">
-        <v>2645</v>
+        <v>0</v>
       </c>
       <c r="W96" s="4">
-        <v>2760</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:23" x14ac:dyDescent="0.25">
@@ -7621,70 +7651,70 @@
         <v>1</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D97" s="4">
-        <v>405</v>
+        <v>440</v>
       </c>
       <c r="E97" s="4">
-        <v>760</v>
+        <v>600</v>
       </c>
       <c r="F97" s="4">
-        <v>1140</v>
+        <v>595</v>
       </c>
       <c r="G97" s="4">
-        <v>1135</v>
+        <v>715</v>
       </c>
       <c r="H97" s="4">
+        <v>885</v>
+      </c>
+      <c r="I97" s="4">
+        <v>1065</v>
+      </c>
+      <c r="J97" s="4">
         <v>1205</v>
       </c>
-      <c r="I97" s="4">
-        <v>1340</v>
-      </c>
-      <c r="J97" s="4">
-        <v>1600</v>
-      </c>
       <c r="K97" s="4">
-        <v>1595</v>
+        <v>1355</v>
       </c>
       <c r="L97" s="4">
-        <v>1700</v>
+        <v>1495</v>
       </c>
       <c r="M97" s="4">
-        <v>1935</v>
+        <v>1640</v>
       </c>
       <c r="N97" s="4">
-        <v>1925</v>
+        <v>1750</v>
       </c>
       <c r="O97" s="4">
-        <v>2030</v>
+        <v>1865</v>
       </c>
       <c r="P97" s="4">
-        <v>2225</v>
+        <v>1975</v>
       </c>
       <c r="Q97" s="4">
-        <v>2425</v>
+        <v>2090</v>
       </c>
       <c r="R97" s="4">
-        <v>2260</v>
+        <v>2195</v>
       </c>
       <c r="S97" s="4">
-        <v>2445</v>
+        <v>2310</v>
       </c>
       <c r="T97" s="4">
-        <v>2615</v>
+        <v>2415</v>
       </c>
       <c r="U97" s="4">
-        <v>2705</v>
+        <v>2530</v>
       </c>
       <c r="V97" s="4">
-        <v>2795</v>
+        <v>2645</v>
       </c>
       <c r="W97" s="4">
-        <v>2890</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="98" spans="1:23" x14ac:dyDescent="0.25">
@@ -7692,70 +7722,70 @@
         <v>1</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D98" s="4">
-        <v>450</v>
+        <v>405</v>
       </c>
       <c r="E98" s="4">
-        <v>845</v>
+        <v>760</v>
       </c>
       <c r="F98" s="4">
-        <v>1270</v>
+        <v>1140</v>
       </c>
       <c r="G98" s="4">
-        <v>0</v>
+        <v>1135</v>
       </c>
       <c r="H98" s="4">
-        <v>0</v>
+        <v>1205</v>
       </c>
       <c r="I98" s="4">
-        <v>0</v>
+        <v>1340</v>
       </c>
       <c r="J98" s="4">
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="K98" s="4">
-        <v>0</v>
+        <v>1595</v>
       </c>
       <c r="L98" s="4">
-        <v>0</v>
+        <v>1700</v>
       </c>
       <c r="M98" s="4">
-        <v>0</v>
+        <v>1935</v>
       </c>
       <c r="N98" s="4">
-        <v>0</v>
+        <v>1925</v>
       </c>
       <c r="O98" s="4">
-        <v>0</v>
+        <v>2030</v>
       </c>
       <c r="P98" s="4">
-        <v>0</v>
+        <v>2225</v>
       </c>
       <c r="Q98" s="4">
-        <v>0</v>
+        <v>2425</v>
       </c>
       <c r="R98" s="4">
-        <v>0</v>
+        <v>2260</v>
       </c>
       <c r="S98" s="4">
-        <v>0</v>
+        <v>2445</v>
       </c>
       <c r="T98" s="4">
-        <v>0</v>
+        <v>2615</v>
       </c>
       <c r="U98" s="4">
-        <v>0</v>
+        <v>2705</v>
       </c>
       <c r="V98" s="4">
-        <v>0</v>
+        <v>2795</v>
       </c>
       <c r="W98" s="4">
-        <v>0</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="99" spans="1:23" x14ac:dyDescent="0.25">
@@ -7763,141 +7793,141 @@
         <v>1</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D99" s="4">
-        <v>355</v>
+        <v>450</v>
       </c>
       <c r="E99" s="4">
-        <v>660</v>
+        <v>845</v>
       </c>
       <c r="F99" s="4">
-        <v>995</v>
+        <v>1270</v>
       </c>
       <c r="G99" s="4">
-        <v>1075</v>
+        <v>0</v>
       </c>
       <c r="H99" s="4">
-        <v>1160</v>
+        <v>0</v>
       </c>
       <c r="I99" s="4">
-        <v>1290</v>
+        <v>0</v>
       </c>
       <c r="J99" s="4">
-        <v>1530</v>
+        <v>0</v>
       </c>
       <c r="K99" s="4">
-        <v>1560</v>
+        <v>0</v>
       </c>
       <c r="L99" s="4">
-        <v>1665</v>
+        <v>0</v>
       </c>
       <c r="M99" s="4">
-        <v>1885</v>
+        <v>0</v>
       </c>
       <c r="N99" s="4">
-        <v>1900</v>
+        <v>0</v>
       </c>
       <c r="O99" s="4">
-        <v>2005</v>
+        <v>0</v>
       </c>
       <c r="P99" s="4">
-        <v>2185</v>
+        <v>0</v>
       </c>
       <c r="Q99" s="4">
-        <v>2390</v>
+        <v>0</v>
       </c>
       <c r="R99" s="4">
-        <v>2230</v>
+        <v>0</v>
       </c>
       <c r="S99" s="4">
-        <v>2410</v>
+        <v>0</v>
       </c>
       <c r="T99" s="4">
-        <v>2580</v>
+        <v>0</v>
       </c>
       <c r="U99" s="4">
-        <v>2755</v>
+        <v>0</v>
       </c>
       <c r="V99" s="4">
-        <v>2935</v>
+        <v>0</v>
       </c>
       <c r="W99" s="4">
-        <v>3115</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="C100" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D100" s="4">
-        <v>460</v>
+        <v>355</v>
       </c>
       <c r="E100" s="4">
-        <v>835</v>
+        <v>660</v>
       </c>
       <c r="F100" s="4">
-        <v>1260</v>
+        <v>995</v>
       </c>
       <c r="G100" s="4">
-        <v>0</v>
+        <v>1075</v>
       </c>
       <c r="H100" s="4">
-        <v>0</v>
+        <v>1160</v>
       </c>
       <c r="I100" s="4">
-        <v>0</v>
+        <v>1290</v>
       </c>
       <c r="J100" s="4">
-        <v>0</v>
+        <v>1530</v>
       </c>
       <c r="K100" s="4">
-        <v>0</v>
+        <v>1560</v>
       </c>
       <c r="L100" s="4">
-        <v>0</v>
+        <v>1665</v>
       </c>
       <c r="M100" s="4">
-        <v>0</v>
+        <v>1885</v>
       </c>
       <c r="N100" s="4">
-        <v>0</v>
+        <v>1900</v>
       </c>
       <c r="O100" s="4">
-        <v>0</v>
+        <v>2005</v>
       </c>
       <c r="P100" s="4">
-        <v>0</v>
+        <v>2185</v>
       </c>
       <c r="Q100" s="4">
-        <v>0</v>
+        <v>2390</v>
       </c>
       <c r="R100" s="4">
-        <v>0</v>
+        <v>2230</v>
       </c>
       <c r="S100" s="4">
-        <v>0</v>
+        <v>2410</v>
       </c>
       <c r="T100" s="4">
-        <v>0</v>
+        <v>2580</v>
       </c>
       <c r="U100" s="4">
-        <v>0</v>
+        <v>2755</v>
       </c>
       <c r="V100" s="4">
-        <v>0</v>
+        <v>2935</v>
       </c>
       <c r="W100" s="4">
-        <v>0</v>
+        <v>3115</v>
       </c>
     </row>
     <row r="101" spans="1:23" x14ac:dyDescent="0.25">
@@ -7905,19 +7935,19 @@
         <v>0</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D101" s="4">
-        <v>370</v>
+        <v>460</v>
       </c>
       <c r="E101" s="4">
-        <v>665</v>
+        <v>835</v>
       </c>
       <c r="F101" s="4">
-        <v>1005</v>
+        <v>1260</v>
       </c>
       <c r="G101" s="4">
         <v>0</v>
@@ -7976,19 +8006,19 @@
         <v>0</v>
       </c>
       <c r="B102" s="11" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D102" s="4">
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="E102" s="4">
-        <v>645</v>
+        <v>665</v>
       </c>
       <c r="F102" s="4">
-        <v>975</v>
+        <v>1005</v>
       </c>
       <c r="G102" s="4">
         <v>0</v>
@@ -8047,19 +8077,19 @@
         <v>0</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D103" s="4">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="E103" s="4">
-        <v>665</v>
+        <v>645</v>
       </c>
       <c r="F103" s="4">
-        <v>1005</v>
+        <v>975</v>
       </c>
       <c r="G103" s="4">
         <v>0</v>
@@ -8118,19 +8148,19 @@
         <v>0</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D104" s="4">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="E104" s="4">
-        <v>650</v>
+        <v>665</v>
       </c>
       <c r="F104" s="4">
-        <v>980</v>
+        <v>1005</v>
       </c>
       <c r="G104" s="4">
         <v>0</v>
@@ -8189,19 +8219,19 @@
         <v>0</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D105" s="4">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="E105" s="4">
-        <v>640</v>
+        <v>650</v>
       </c>
       <c r="F105" s="4">
-        <v>955</v>
+        <v>980</v>
       </c>
       <c r="G105" s="4">
         <v>0</v>
@@ -8260,19 +8290,19 @@
         <v>0</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="C106" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D106" s="4">
-        <v>365</v>
+        <v>340</v>
       </c>
       <c r="E106" s="4">
-        <v>695</v>
+        <v>640</v>
       </c>
       <c r="F106" s="4">
-        <v>1040</v>
+        <v>955</v>
       </c>
       <c r="G106" s="4">
         <v>0</v>
@@ -8331,19 +8361,19 @@
         <v>0</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D107" s="4">
-        <v>240</v>
+        <v>365</v>
       </c>
       <c r="E107" s="4">
-        <v>405</v>
+        <v>695</v>
       </c>
       <c r="F107" s="4">
-        <v>600</v>
+        <v>1040</v>
       </c>
       <c r="G107" s="4">
         <v>0</v>
@@ -8402,69 +8432,140 @@
         <v>0</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="C108" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D108" s="4">
+        <v>240</v>
+      </c>
+      <c r="E108" s="4">
+        <v>405</v>
+      </c>
+      <c r="F108" s="4">
+        <v>600</v>
+      </c>
+      <c r="G108" s="4">
+        <v>0</v>
+      </c>
+      <c r="H108" s="4">
+        <v>0</v>
+      </c>
+      <c r="I108" s="4">
+        <v>0</v>
+      </c>
+      <c r="J108" s="4">
+        <v>0</v>
+      </c>
+      <c r="K108" s="4">
+        <v>0</v>
+      </c>
+      <c r="L108" s="4">
+        <v>0</v>
+      </c>
+      <c r="M108" s="4">
+        <v>0</v>
+      </c>
+      <c r="N108" s="4">
+        <v>0</v>
+      </c>
+      <c r="O108" s="4">
+        <v>0</v>
+      </c>
+      <c r="P108" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q108" s="4">
+        <v>0</v>
+      </c>
+      <c r="R108" s="4">
+        <v>0</v>
+      </c>
+      <c r="S108" s="4">
+        <v>0</v>
+      </c>
+      <c r="T108" s="4">
+        <v>0</v>
+      </c>
+      <c r="U108" s="4">
+        <v>0</v>
+      </c>
+      <c r="V108" s="4">
+        <v>0</v>
+      </c>
+      <c r="W108" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A109" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D109" s="4">
         <v>435</v>
       </c>
-      <c r="E108" s="4">
+      <c r="E109" s="4">
         <v>825</v>
       </c>
-      <c r="F108" s="4">
+      <c r="F109" s="4">
         <v>1240</v>
       </c>
-      <c r="G108" s="4">
-        <v>0</v>
-      </c>
-      <c r="H108" s="4">
-        <v>0</v>
-      </c>
-      <c r="I108" s="4">
-        <v>0</v>
-      </c>
-      <c r="J108" s="4">
-        <v>0</v>
-      </c>
-      <c r="K108" s="4">
-        <v>0</v>
-      </c>
-      <c r="L108" s="4">
-        <v>0</v>
-      </c>
-      <c r="M108" s="4">
-        <v>0</v>
-      </c>
-      <c r="N108" s="4">
-        <v>0</v>
-      </c>
-      <c r="O108" s="4">
-        <v>0</v>
-      </c>
-      <c r="P108" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q108" s="4">
-        <v>0</v>
-      </c>
-      <c r="R108" s="4">
-        <v>0</v>
-      </c>
-      <c r="S108" s="4">
-        <v>0</v>
-      </c>
-      <c r="T108" s="4">
-        <v>0</v>
-      </c>
-      <c r="U108" s="4">
-        <v>0</v>
-      </c>
-      <c r="V108" s="4">
-        <v>0</v>
-      </c>
-      <c r="W108" s="4">
+      <c r="G109" s="4">
+        <v>0</v>
+      </c>
+      <c r="H109" s="4">
+        <v>0</v>
+      </c>
+      <c r="I109" s="4">
+        <v>0</v>
+      </c>
+      <c r="J109" s="4">
+        <v>0</v>
+      </c>
+      <c r="K109" s="4">
+        <v>0</v>
+      </c>
+      <c r="L109" s="4">
+        <v>0</v>
+      </c>
+      <c r="M109" s="4">
+        <v>0</v>
+      </c>
+      <c r="N109" s="4">
+        <v>0</v>
+      </c>
+      <c r="O109" s="4">
+        <v>0</v>
+      </c>
+      <c r="P109" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q109" s="4">
+        <v>0</v>
+      </c>
+      <c r="R109" s="4">
+        <v>0</v>
+      </c>
+      <c r="S109" s="4">
+        <v>0</v>
+      </c>
+      <c r="T109" s="4">
+        <v>0</v>
+      </c>
+      <c r="U109" s="4">
+        <v>0</v>
+      </c>
+      <c r="V109" s="4">
+        <v>0</v>
+      </c>
+      <c r="W109" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>